<commit_message>
updated bracket display on edit players page
</commit_message>
<xml_diff>
--- a/form_design/Bracket Merge.xlsx
+++ b/form_design/Bracket Merge.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects 2017\Codecademy\Portfolio\bowl_tmnts\form_design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABCE1DC-63EC-4162-B7EE-22ABB68C541F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8897D16-F1BE-441A-9B56-ECD6E2990AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="6" xr2:uid="{A2505C3C-2350-4FE2-AF4A-826C0074D70B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="12" xr2:uid="{A2505C3C-2350-4FE2-AF4A-826C0074D70B}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate Full and Bye" sheetId="13" r:id="rId1"/>
     <sheet name="Initial Data" sheetId="16" r:id="rId2"/>
     <sheet name="1 Player 10 Rest 4" sheetId="19" r:id="rId3"/>
     <sheet name="10 Players 10 Each" sheetId="21" r:id="rId4"/>
-    <sheet name="14 Players" sheetId="17" r:id="rId5"/>
+    <sheet name="12 Players" sheetId="17" r:id="rId5"/>
     <sheet name="EdgeCase1 1P-All Brkts" sheetId="14" r:id="rId6"/>
     <sheet name="EdgeCase2 2P-All Brkts" sheetId="15" r:id="rId7"/>
     <sheet name="EdgeCase3 10Px4B" sheetId="18" r:id="rId8"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2571" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2572" uniqueCount="120">
   <si>
     <t>Pos</t>
   </si>
@@ -408,6 +408,9 @@
   <si>
     <t xml:space="preserve">Random </t>
   </si>
+  <si>
+    <t>OLD CODE</t>
+  </si>
 </sst>
 </file>
 
@@ -644,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -751,29 +754,28 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1125,7 +1127,7 @@
   <dimension ref="A1:AD21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Y10" sqref="Y10:AD10"/>
+      <selection activeCell="AD16" sqref="U16:AD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,30 +1144,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="54"/>
-      <c r="I1" s="52" t="s">
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="52"/>
+      <c r="I1" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="52"/>
-      <c r="L1" s="55" t="s">
+      <c r="J1" s="57"/>
+      <c r="L1" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
     </row>
     <row r="2" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -1947,7 +1949,7 @@
       <c r="J12" s="46">
         <v>8</v>
       </c>
-      <c r="L12" s="60" t="s">
+      <c r="L12" s="55" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1983,14 +1985,14 @@
       <c r="B14" s="34">
         <v>5</v>
       </c>
-      <c r="E14" s="57">
-        <v>12</v>
-      </c>
-      <c r="F14" s="57">
+      <c r="E14" s="53">
+        <v>12</v>
+      </c>
+      <c r="F14" s="53">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G14" s="57">
+      <c r="G14" s="53">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
@@ -2189,7 +2191,7 @@
       <c r="J17" s="6">
         <v>5</v>
       </c>
-      <c r="L17" s="60" t="s">
+      <c r="L17" s="55" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2337,7 +2339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C0A208A-0182-4269-A4D1-89FEA39E88E1}">
   <dimension ref="A1:AH21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="P9" sqref="P9:R9"/>
     </sheetView>
   </sheetViews>
@@ -2360,42 +2362,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="I1" s="55" t="s">
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="I1" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="55"/>
-      <c r="L1" s="56" t="s">
+      <c r="J1" s="58"/>
+      <c r="L1" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="W1" s="55" t="s">
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="W1" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
-      <c r="AD1" s="55"/>
-      <c r="AE1" s="55"/>
-      <c r="AF1" s="55"/>
-      <c r="AG1" s="55"/>
-      <c r="AH1" s="55"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
+      <c r="Z1" s="58"/>
+      <c r="AA1" s="58"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="58"/>
+      <c r="AD1" s="58"/>
+      <c r="AE1" s="58"/>
+      <c r="AF1" s="58"/>
+      <c r="AG1" s="58"/>
+      <c r="AH1" s="58"/>
     </row>
     <row r="2" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -2997,14 +2999,14 @@
       <c r="B9" s="19">
         <v>10</v>
       </c>
-      <c r="E9" s="57">
+      <c r="E9" s="53">
         <v>7</v>
       </c>
-      <c r="F9" s="57">
+      <c r="F9" s="53">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G9" s="57">
+      <c r="G9" s="53">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
@@ -3179,7 +3181,7 @@
         <f t="shared" si="3"/>
         <v>8.5714285714285712</v>
       </c>
-      <c r="W12" s="60" t="s">
+      <c r="W12" s="55" t="s">
         <v>102</v>
       </c>
     </row>
@@ -3403,7 +3405,7 @@
         <f t="shared" si="3"/>
         <v>7.8571428571428568</v>
       </c>
-      <c r="W17" s="60" t="s">
+      <c r="W17" s="55" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3594,42 +3596,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="I1" s="55" t="s">
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="I1" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="55"/>
-      <c r="L1" s="56" t="s">
+      <c r="J1" s="58"/>
+      <c r="L1" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="W1" s="55" t="s">
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="W1" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
-      <c r="AD1" s="55"/>
-      <c r="AE1" s="55"/>
-      <c r="AF1" s="55"/>
-      <c r="AG1" s="55"/>
-      <c r="AH1" s="55"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
+      <c r="Z1" s="58"/>
+      <c r="AA1" s="58"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="58"/>
+      <c r="AD1" s="58"/>
+      <c r="AE1" s="58"/>
+      <c r="AF1" s="58"/>
+      <c r="AG1" s="58"/>
+      <c r="AH1" s="58"/>
     </row>
     <row r="2" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -4329,7 +4331,7 @@
         <f t="shared" si="3"/>
         <v>2.5714285714285712</v>
       </c>
-      <c r="W12" s="60" t="s">
+      <c r="W12" s="55" t="s">
         <v>102</v>
       </c>
     </row>
@@ -4553,7 +4555,7 @@
         <f t="shared" si="3"/>
         <v>1.8571428571428577</v>
       </c>
-      <c r="W17" s="60" t="s">
+      <c r="W17" s="55" t="s">
         <v>101</v>
       </c>
     </row>
@@ -4744,42 +4746,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="I1" s="55" t="s">
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="I1" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="55"/>
-      <c r="L1" s="56" t="s">
+      <c r="J1" s="58"/>
+      <c r="L1" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="W1" s="55" t="s">
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="W1" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
-      <c r="AD1" s="55"/>
-      <c r="AE1" s="55"/>
-      <c r="AF1" s="55"/>
-      <c r="AG1" s="55"/>
-      <c r="AH1" s="55"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
+      <c r="Z1" s="58"/>
+      <c r="AA1" s="58"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="58"/>
+      <c r="AD1" s="58"/>
+      <c r="AE1" s="58"/>
+      <c r="AF1" s="58"/>
+      <c r="AG1" s="58"/>
+      <c r="AH1" s="58"/>
     </row>
     <row r="2" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -5493,7 +5495,7 @@
         <f t="shared" si="3"/>
         <v>3.5714285714285712</v>
       </c>
-      <c r="W12" s="60" t="s">
+      <c r="W12" s="55" t="s">
         <v>102</v>
       </c>
     </row>
@@ -5717,7 +5719,7 @@
         <f t="shared" si="3"/>
         <v>2.8571428571428577</v>
       </c>
-      <c r="W17" s="60" t="s">
+      <c r="W17" s="55" t="s">
         <v>101</v>
       </c>
     </row>
@@ -5888,8 +5890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF879227-BB89-4EAE-A811-B9676B93970D}">
   <dimension ref="A1:AP24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5911,42 +5913,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="I1" s="55" t="s">
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="I1" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="55"/>
-      <c r="L1" s="56" t="s">
+      <c r="J1" s="58"/>
+      <c r="L1" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="W1" s="55" t="s">
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="W1" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
-      <c r="AD1" s="55"/>
-      <c r="AE1" s="55"/>
-      <c r="AF1" s="55"/>
-      <c r="AG1" s="55"/>
-      <c r="AH1" s="55"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
+      <c r="Z1" s="58"/>
+      <c r="AA1" s="58"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="58"/>
+      <c r="AD1" s="58"/>
+      <c r="AE1" s="58"/>
+      <c r="AF1" s="58"/>
+      <c r="AG1" s="58"/>
+      <c r="AH1" s="58"/>
     </row>
     <row r="2" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -6764,7 +6766,7 @@
       <c r="U12" s="27">
         <v>1</v>
       </c>
-      <c r="W12" s="60" t="s">
+      <c r="W12" s="55" t="s">
         <v>102</v>
       </c>
     </row>
@@ -6833,19 +6835,19 @@
         <v>77</v>
       </c>
       <c r="X14" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y14" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z14" s="16">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="AA14" s="16">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="AB14" s="16">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="AC14" s="16">
         <v>8</v>
@@ -6903,13 +6905,13 @@
         <v>0</v>
       </c>
       <c r="Z15" s="16">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AA15" s="16">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AB15" s="16">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AC15" s="16">
         <v>7</v>
@@ -6988,7 +6990,7 @@
         <f t="shared" si="3"/>
         <v>0.14285714285714235</v>
       </c>
-      <c r="W17" s="60" t="s">
+      <c r="W17" s="55" t="s">
         <v>101</v>
       </c>
     </row>
@@ -7155,7 +7157,7 @@
       </c>
       <c r="B23" s="1">
         <f ca="1">INT((RAND()*10)+1)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="W23" t="s">
         <v>79</v>
@@ -7210,42 +7212,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="I1" s="55" t="s">
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="I1" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="55"/>
-      <c r="L1" s="56" t="s">
+      <c r="J1" s="58"/>
+      <c r="L1" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="W1" s="55" t="s">
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="W1" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
-      <c r="AD1" s="55"/>
-      <c r="AE1" s="55"/>
-      <c r="AF1" s="55"/>
-      <c r="AG1" s="55"/>
-      <c r="AH1" s="55"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
+      <c r="Z1" s="58"/>
+      <c r="AA1" s="58"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="58"/>
+      <c r="AD1" s="58"/>
+      <c r="AE1" s="58"/>
+      <c r="AF1" s="58"/>
+      <c r="AG1" s="58"/>
+      <c r="AH1" s="58"/>
     </row>
     <row r="2" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -8047,7 +8049,7 @@
         <f t="shared" si="3"/>
         <v>3.5714285714285712</v>
       </c>
-      <c r="W12" s="60" t="s">
+      <c r="W12" s="55" t="s">
         <v>102</v>
       </c>
     </row>
@@ -8271,7 +8273,7 @@
         <f t="shared" si="3"/>
         <v>2.8571428571428577</v>
       </c>
-      <c r="W17" s="60" t="s">
+      <c r="W17" s="55" t="s">
         <v>101</v>
       </c>
     </row>
@@ -8438,7 +8440,7 @@
       </c>
       <c r="B23" s="1">
         <f ca="1">INT((RAND()*10)+1)</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="W23" t="s">
         <v>79</v>
@@ -8474,7 +8476,7 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V35" sqref="V35"/>
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8497,6 +8499,10 @@
       <c r="O1" s="30">
         <v>15</v>
       </c>
+      <c r="Q1" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="R1" s="55"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -10015,7 +10021,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10040,30 +10046,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="54"/>
-      <c r="I1" s="52" t="s">
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="52"/>
+      <c r="I1" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="52"/>
-      <c r="L1" s="55" t="s">
+      <c r="J1" s="57"/>
+      <c r="L1" s="58" t="s">
         <v>105</v>
       </c>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -10571,7 +10577,7 @@
       <c r="L10" s="16">
         <v>8</v>
       </c>
-      <c r="M10" s="58" t="s">
+      <c r="M10" s="28" t="s">
         <v>24</v>
       </c>
       <c r="N10" s="28" t="s">
@@ -10635,14 +10641,14 @@
       <c r="B12" s="27">
         <v>10</v>
       </c>
-      <c r="E12" s="57">
+      <c r="E12" s="53">
         <v>10</v>
       </c>
-      <c r="F12" s="57">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="57">
+      <c r="F12" s="53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="53">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
@@ -10652,7 +10658,7 @@
       <c r="J12" s="29">
         <v>6</v>
       </c>
-      <c r="L12" s="60" t="s">
+      <c r="L12" s="55" t="s">
         <v>102</v>
       </c>
     </row>
@@ -10822,7 +10828,7 @@
         <f t="shared" si="1"/>
         <v>9.2857142857142847</v>
       </c>
-      <c r="L17" s="60" t="s">
+      <c r="L17" s="55" t="s">
         <v>101</v>
       </c>
     </row>
@@ -10952,7 +10958,7 @@
   <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:G10"/>
+      <selection activeCell="C4" sqref="C4:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10969,30 +10975,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="54"/>
-      <c r="I1" s="52" t="s">
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="52"/>
+      <c r="I1" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="52"/>
-      <c r="L1" s="55" t="s">
+      <c r="J1" s="57"/>
+      <c r="L1" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -11480,14 +11486,14 @@
       <c r="B10" s="23">
         <v>4</v>
       </c>
-      <c r="E10" s="57">
+      <c r="E10" s="53">
         <v>8</v>
       </c>
-      <c r="F10" s="57">
+      <c r="F10" s="53">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G10" s="57">
+      <c r="G10" s="53">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
@@ -11577,7 +11583,7 @@
       <c r="J12" s="27">
         <v>4</v>
       </c>
-      <c r="L12" s="60" t="s">
+      <c r="L12" s="55" t="s">
         <v>102</v>
       </c>
     </row>
@@ -11771,7 +11777,7 @@
       <c r="J17" s="41">
         <v>4</v>
       </c>
-      <c r="L17" s="60" t="s">
+      <c r="L17" s="55" t="s">
         <v>101</v>
       </c>
     </row>
@@ -11919,7 +11925,7 @@
   <dimension ref="A1:Y21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:G11"/>
+      <selection activeCell="Y13" sqref="P13:Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11936,30 +11942,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="54"/>
-      <c r="I1" s="52" t="s">
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="52"/>
+      <c r="I1" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="52"/>
-      <c r="L1" s="55" t="s">
+      <c r="J1" s="57"/>
+      <c r="L1" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -12568,14 +12574,14 @@
       <c r="B11" s="25">
         <v>10</v>
       </c>
-      <c r="E11" s="57">
+      <c r="E11" s="53">
         <v>9</v>
       </c>
-      <c r="F11" s="57">
+      <c r="F11" s="53">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G11" s="57">
+      <c r="G11" s="53">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
@@ -12610,7 +12616,7 @@
       <c r="J12" s="27">
         <v>10</v>
       </c>
-      <c r="L12" s="60" t="s">
+      <c r="L12" s="55" t="s">
         <v>102</v>
       </c>
     </row>
@@ -12792,7 +12798,7 @@
         <f t="shared" si="1"/>
         <v>12.142857142857142</v>
       </c>
-      <c r="L17" s="60" t="s">
+      <c r="L17" s="55" t="s">
         <v>101</v>
       </c>
     </row>
@@ -12919,7 +12925,7 @@
   <dimension ref="A1:Y21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K10"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12936,30 +12942,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="54"/>
-      <c r="I1" s="52" t="s">
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="52"/>
+      <c r="I1" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="52"/>
-      <c r="L1" s="55" t="s">
+      <c r="J1" s="57"/>
+      <c r="L1" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -13568,14 +13574,14 @@
       <c r="B11" s="25">
         <v>5</v>
       </c>
-      <c r="E11" s="57">
+      <c r="E11" s="53">
         <v>9</v>
       </c>
-      <c r="F11" s="57">
+      <c r="F11" s="53">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G11" s="57">
+      <c r="G11" s="53">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
@@ -13610,7 +13616,7 @@
       <c r="J12" s="27">
         <v>5</v>
       </c>
-      <c r="L12" s="60" t="s">
+      <c r="L12" s="55" t="s">
         <v>102</v>
       </c>
     </row>
@@ -13804,7 +13810,7 @@
         <f t="shared" si="1"/>
         <v>12.142857142857142</v>
       </c>
-      <c r="L17" s="60" t="s">
+      <c r="L17" s="55" t="s">
         <v>101</v>
       </c>
     </row>
@@ -13931,7 +13937,7 @@
   <dimension ref="A1:AP22"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="AP13" sqref="AG13:AP13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13953,42 +13959,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="I1" s="55" t="s">
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="I1" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="55"/>
-      <c r="L1" s="56" t="s">
+      <c r="J1" s="58"/>
+      <c r="L1" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="W1" s="55" t="s">
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="W1" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
-      <c r="AD1" s="55"/>
-      <c r="AE1" s="55"/>
-      <c r="AF1" s="55"/>
-      <c r="AG1" s="55"/>
-      <c r="AH1" s="55"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
+      <c r="Z1" s="58"/>
+      <c r="AA1" s="58"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="58"/>
+      <c r="AD1" s="58"/>
+      <c r="AE1" s="58"/>
+      <c r="AF1" s="58"/>
+      <c r="AG1" s="58"/>
+      <c r="AH1" s="58"/>
     </row>
     <row r="2" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -15068,7 +15074,7 @@
       <c r="U12" s="46">
         <v>8</v>
       </c>
-      <c r="W12" s="60" t="s">
+      <c r="W12" s="55" t="s">
         <v>102</v>
       </c>
     </row>
@@ -15370,14 +15376,14 @@
         <v>10</v>
       </c>
       <c r="N16"/>
-      <c r="P16" s="57">
+      <c r="P16" s="53">
         <v>14</v>
       </c>
-      <c r="Q16" s="57">
+      <c r="Q16" s="53">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="R16" s="57">
+      <c r="R16" s="53">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
@@ -15436,7 +15442,7 @@
       <c r="U17" s="6">
         <v>5</v>
       </c>
-      <c r="W17" s="60" t="s">
+      <c r="W17" s="55" t="s">
         <v>101</v>
       </c>
     </row>
@@ -15496,14 +15502,14 @@
       <c r="B19" s="43">
         <v>5</v>
       </c>
-      <c r="E19" s="59">
+      <c r="E19" s="54">
         <v>17</v>
       </c>
-      <c r="F19" s="59">
+      <c r="F19" s="54">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G19" s="59">
+      <c r="G19" s="54">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
@@ -15686,8 +15692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E221FD3C-92F6-4A66-8405-D689C910F205}">
   <dimension ref="A1:AR33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AR10" sqref="AR10"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AR13" sqref="AI13:AR13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15709,42 +15715,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="54"/>
-      <c r="I1" s="55" t="s">
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="52"/>
+      <c r="I1" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="55"/>
-      <c r="L1" s="56" t="s">
+      <c r="J1" s="58"/>
+      <c r="L1" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="W1" s="55" t="s">
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="W1" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
-      <c r="AD1" s="55"/>
-      <c r="AE1" s="55"/>
-      <c r="AF1" s="55"/>
-      <c r="AG1" s="55"/>
-      <c r="AH1" s="55"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
+      <c r="Z1" s="58"/>
+      <c r="AA1" s="58"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="58"/>
+      <c r="AD1" s="58"/>
+      <c r="AE1" s="58"/>
+      <c r="AF1" s="58"/>
+      <c r="AG1" s="58"/>
+      <c r="AH1" s="58"/>
     </row>
     <row r="2" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -15895,23 +15901,23 @@
         <v>12</v>
       </c>
       <c r="M3" s="21">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="N3"/>
       <c r="O3" s="1">
         <f>SUM(M3:M20)</f>
-        <v>198</v>
+        <v>162</v>
       </c>
       <c r="P3" s="1">
         <v>1</v>
       </c>
       <c r="Q3" s="1">
         <f>($O$3-(8*P3))/7</f>
-        <v>27.142857142857142</v>
+        <v>22</v>
       </c>
       <c r="R3" s="1">
         <f>P3+Q3</f>
-        <v>28.142857142857142</v>
+        <v>23</v>
       </c>
       <c r="T3" s="20" t="s">
         <v>12</v>
@@ -16014,7 +16020,7 @@
         <v>13</v>
       </c>
       <c r="M4" s="4">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="N4"/>
       <c r="P4" s="1">
@@ -16022,11 +16028,11 @@
       </c>
       <c r="Q4" s="1">
         <f t="shared" ref="Q4:Q33" si="2">($O$3-(8*P4))/7</f>
-        <v>26</v>
+        <v>20.857142857142858</v>
       </c>
       <c r="R4" s="1">
         <f t="shared" ref="R4:R33" si="3">P4+Q4</f>
-        <v>28</v>
+        <v>22.857142857142858</v>
       </c>
       <c r="T4" s="3" t="s">
         <v>13</v>
@@ -16137,11 +16143,11 @@
       </c>
       <c r="Q5" s="1">
         <f t="shared" si="2"/>
-        <v>24.857142857142858</v>
+        <v>19.714285714285715</v>
       </c>
       <c r="R5" s="1">
         <f t="shared" si="3"/>
-        <v>27.857142857142858</v>
+        <v>22.714285714285715</v>
       </c>
       <c r="T5" s="10" t="s">
         <v>16</v>
@@ -16252,11 +16258,11 @@
       </c>
       <c r="Q6" s="1">
         <f t="shared" si="2"/>
-        <v>23.714285714285715</v>
+        <v>18.571428571428573</v>
       </c>
       <c r="R6" s="1">
         <f t="shared" si="3"/>
-        <v>27.714285714285715</v>
+        <v>22.571428571428573</v>
       </c>
       <c r="T6" s="8" t="s">
         <v>15</v>
@@ -16367,11 +16373,11 @@
       </c>
       <c r="Q7" s="1">
         <f t="shared" si="2"/>
-        <v>22.571428571428573</v>
+        <v>17.428571428571427</v>
       </c>
       <c r="R7" s="1">
         <f t="shared" si="3"/>
-        <v>27.571428571428573</v>
+        <v>22.428571428571427</v>
       </c>
       <c r="T7" s="26" t="s">
         <v>23</v>
@@ -16482,11 +16488,11 @@
       </c>
       <c r="Q8" s="1">
         <f t="shared" si="2"/>
-        <v>21.428571428571427</v>
+        <v>16.285714285714285</v>
       </c>
       <c r="R8" s="1">
         <f t="shared" si="3"/>
-        <v>27.428571428571427</v>
+        <v>22.285714285714285</v>
       </c>
       <c r="T8" s="35" t="s">
         <v>72</v>
@@ -16597,11 +16603,11 @@
       </c>
       <c r="Q9" s="1">
         <f t="shared" si="2"/>
-        <v>20.285714285714285</v>
+        <v>15.142857142857142</v>
       </c>
       <c r="R9" s="1">
         <f t="shared" si="3"/>
-        <v>27.285714285714285</v>
+        <v>22.142857142857142</v>
       </c>
       <c r="T9" s="39" t="s">
         <v>76</v>
@@ -16712,11 +16718,11 @@
       </c>
       <c r="Q10" s="1">
         <f t="shared" si="2"/>
-        <v>19.142857142857142</v>
+        <v>14</v>
       </c>
       <c r="R10" s="1">
         <f t="shared" si="3"/>
-        <v>27.142857142857142</v>
+        <v>22</v>
       </c>
       <c r="T10" s="22" t="s">
         <v>19</v>
@@ -16815,11 +16821,11 @@
       </c>
       <c r="Q11" s="1">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>12.857142857142858</v>
       </c>
       <c r="R11" s="1">
         <f t="shared" si="3"/>
-        <v>27</v>
+        <v>21.857142857142858</v>
       </c>
       <c r="T11" s="24" t="s">
         <v>22</v>
@@ -16864,11 +16870,11 @@
       </c>
       <c r="Q12" s="1">
         <f t="shared" si="2"/>
-        <v>16.857142857142858</v>
+        <v>11.714285714285714</v>
       </c>
       <c r="R12" s="1">
         <f t="shared" si="3"/>
-        <v>26.857142857142858</v>
+        <v>21.714285714285715</v>
       </c>
       <c r="T12" s="45" t="s">
         <v>71</v>
@@ -16876,7 +16882,7 @@
       <c r="U12" s="46">
         <v>8</v>
       </c>
-      <c r="W12" s="60" t="s">
+      <c r="W12" s="55" t="s">
         <v>102</v>
       </c>
     </row>
@@ -16916,11 +16922,11 @@
       </c>
       <c r="Q13" s="1">
         <f t="shared" si="2"/>
-        <v>15.714285714285714</v>
+        <v>10.571428571428571</v>
       </c>
       <c r="R13" s="1">
         <f t="shared" si="3"/>
-        <v>26.714285714285715</v>
+        <v>21.571428571428569</v>
       </c>
       <c r="T13" s="36" t="s">
         <v>73</v>
@@ -16965,11 +16971,11 @@
       </c>
       <c r="Q14" s="1">
         <f t="shared" si="2"/>
-        <v>14.571428571428571</v>
+        <v>9.4285714285714288</v>
       </c>
       <c r="R14" s="1">
         <f t="shared" si="3"/>
-        <v>26.571428571428569</v>
+        <v>21.428571428571431</v>
       </c>
       <c r="T14" s="12" t="s">
         <v>17</v>
@@ -17080,11 +17086,11 @@
       </c>
       <c r="Q15" s="1">
         <f t="shared" si="2"/>
-        <v>13.428571428571429</v>
+        <v>8.2857142857142865</v>
       </c>
       <c r="R15" s="1">
         <f t="shared" si="3"/>
-        <v>26.428571428571431</v>
+        <v>21.285714285714285</v>
       </c>
       <c r="T15" s="18" t="s">
         <v>18</v>
@@ -17195,11 +17201,11 @@
       </c>
       <c r="Q16" s="1">
         <f t="shared" si="2"/>
-        <v>12.285714285714286</v>
+        <v>7.1428571428571432</v>
       </c>
       <c r="R16" s="1">
         <f t="shared" si="3"/>
-        <v>26.285714285714285</v>
+        <v>21.142857142857142</v>
       </c>
       <c r="T16" s="32" t="s">
         <v>24</v>
@@ -17239,16 +17245,16 @@
         <v>7</v>
       </c>
       <c r="N17"/>
-      <c r="P17" s="57">
+      <c r="P17" s="53">
         <v>15</v>
       </c>
-      <c r="Q17" s="57">
+      <c r="Q17" s="53">
         <f t="shared" si="2"/>
-        <v>11.142857142857142</v>
-      </c>
-      <c r="R17" s="57">
+        <v>6</v>
+      </c>
+      <c r="R17" s="53">
         <f t="shared" si="3"/>
-        <v>26.142857142857142</v>
+        <v>21</v>
       </c>
       <c r="T17" s="5" t="s">
         <v>14</v>
@@ -17256,7 +17262,7 @@
       <c r="U17" s="6">
         <v>5</v>
       </c>
-      <c r="W17" s="60" t="s">
+      <c r="W17" s="55" t="s">
         <v>101</v>
       </c>
     </row>
@@ -17296,11 +17302,11 @@
       </c>
       <c r="Q18" s="1">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>4.8571428571428568</v>
       </c>
       <c r="R18" s="1">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>20.857142857142858</v>
       </c>
       <c r="T18" s="33" t="s">
         <v>70</v>
@@ -17345,11 +17351,11 @@
       </c>
       <c r="Q19" s="1">
         <f t="shared" si="2"/>
-        <v>8.8571428571428577</v>
+        <v>3.7142857142857144</v>
       </c>
       <c r="R19" s="1">
         <f t="shared" si="3"/>
-        <v>25.857142857142858</v>
+        <v>20.714285714285715</v>
       </c>
       <c r="T19" s="38" t="s">
         <v>75</v>
@@ -17439,11 +17445,11 @@
       </c>
       <c r="Q20" s="1">
         <f t="shared" si="2"/>
-        <v>7.7142857142857144</v>
+        <v>2.5714285714285716</v>
       </c>
       <c r="R20" s="1">
         <f t="shared" si="3"/>
-        <v>25.714285714285715</v>
+        <v>20.571428571428573</v>
       </c>
       <c r="T20" s="37" t="s">
         <v>74</v>
@@ -17471,18 +17477,18 @@
       <c r="L21"/>
       <c r="M21" s="1">
         <f>SUM(M3:M20)</f>
-        <v>198</v>
+        <v>162</v>
       </c>
       <c r="P21" s="1">
         <v>19</v>
       </c>
       <c r="Q21" s="1">
         <f t="shared" si="2"/>
-        <v>6.5714285714285712</v>
+        <v>1.4285714285714286</v>
       </c>
       <c r="R21" s="1">
         <f t="shared" si="3"/>
-        <v>25.571428571428569</v>
+        <v>20.428571428571427</v>
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
@@ -17502,11 +17508,11 @@
       </c>
       <c r="Q22" s="1">
         <f t="shared" si="2"/>
-        <v>5.4285714285714288</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="R22" s="1">
         <f t="shared" si="3"/>
-        <v>25.428571428571431</v>
+        <v>20.285714285714285</v>
       </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
@@ -17526,11 +17532,11 @@
       </c>
       <c r="Q23" s="1">
         <f t="shared" si="2"/>
-        <v>4.2857142857142856</v>
+        <v>-0.8571428571428571</v>
       </c>
       <c r="R23" s="1">
         <f t="shared" si="3"/>
-        <v>25.285714285714285</v>
+        <v>20.142857142857142</v>
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
@@ -17550,11 +17556,11 @@
       </c>
       <c r="Q24" s="1">
         <f t="shared" si="2"/>
-        <v>3.1428571428571428</v>
+        <v>-2</v>
       </c>
       <c r="R24" s="1">
         <f t="shared" si="3"/>
-        <v>25.142857142857142</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
@@ -17574,22 +17580,22 @@
       </c>
       <c r="Q25" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>-3.1428571428571428</v>
       </c>
       <c r="R25" s="1">
         <f t="shared" si="3"/>
-        <v>25</v>
+        <v>19.857142857142858</v>
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="E26" s="59">
+      <c r="E26" s="54">
         <v>24</v>
       </c>
-      <c r="F26" s="59">
+      <c r="F26" s="54">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G26" s="59">
+      <c r="G26" s="54">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
@@ -17598,11 +17604,11 @@
       </c>
       <c r="Q26" s="1">
         <f t="shared" si="2"/>
-        <v>0.8571428571428571</v>
+        <v>-4.2857142857142856</v>
       </c>
       <c r="R26" s="1">
         <f t="shared" si="3"/>
-        <v>24.857142857142858</v>
+        <v>19.714285714285715</v>
       </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
@@ -17622,11 +17628,11 @@
       </c>
       <c r="Q27" s="1">
         <f t="shared" si="2"/>
-        <v>-0.2857142857142857</v>
+        <v>-5.4285714285714288</v>
       </c>
       <c r="R27" s="1">
         <f t="shared" si="3"/>
-        <v>24.714285714285715</v>
+        <v>19.571428571428569</v>
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
@@ -17646,11 +17652,11 @@
       </c>
       <c r="Q28" s="1">
         <f t="shared" si="2"/>
-        <v>-1.4285714285714286</v>
+        <v>-6.5714285714285712</v>
       </c>
       <c r="R28" s="1">
         <f t="shared" si="3"/>
-        <v>24.571428571428573</v>
+        <v>19.428571428571431</v>
       </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
@@ -17670,11 +17676,11 @@
       </c>
       <c r="Q29" s="1">
         <f t="shared" si="2"/>
-        <v>-2.5714285714285716</v>
+        <v>-7.7142857142857144</v>
       </c>
       <c r="R29" s="1">
         <f t="shared" si="3"/>
-        <v>24.428571428571427</v>
+        <v>19.285714285714285</v>
       </c>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.25">
@@ -17694,11 +17700,11 @@
       </c>
       <c r="Q30" s="1">
         <f t="shared" si="2"/>
-        <v>-3.7142857142857144</v>
+        <v>-8.8571428571428577</v>
       </c>
       <c r="R30" s="1">
         <f t="shared" si="3"/>
-        <v>24.285714285714285</v>
+        <v>19.142857142857142</v>
       </c>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.25">
@@ -17718,11 +17724,11 @@
       </c>
       <c r="Q31" s="1">
         <f t="shared" si="2"/>
-        <v>-4.8571428571428568</v>
+        <v>-10</v>
       </c>
       <c r="R31" s="1">
         <f t="shared" si="3"/>
-        <v>24.142857142857142</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
@@ -17742,11 +17748,11 @@
       </c>
       <c r="Q32" s="1">
         <f t="shared" si="2"/>
-        <v>-6</v>
+        <v>-11.142857142857142</v>
       </c>
       <c r="R32" s="1">
         <f t="shared" si="3"/>
-        <v>24</v>
+        <v>18.857142857142858</v>
       </c>
     </row>
     <row r="33" spans="5:18" x14ac:dyDescent="0.25">
@@ -17766,11 +17772,11 @@
       </c>
       <c r="Q33" s="1">
         <f t="shared" si="2"/>
-        <v>-7.1428571428571432</v>
+        <v>-12.285714285714286</v>
       </c>
       <c r="R33" s="1">
         <f t="shared" si="3"/>
-        <v>23.857142857142858</v>
+        <v>18.714285714285715</v>
       </c>
     </row>
   </sheetData>
@@ -17808,30 +17814,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="54"/>
-      <c r="I1" s="52" t="s">
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="52"/>
+      <c r="I1" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="52"/>
-      <c r="L1" s="55" t="s">
+      <c r="J1" s="57"/>
+      <c r="L1" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -18102,14 +18108,14 @@
       <c r="B7" s="11">
         <v>4</v>
       </c>
-      <c r="E7" s="57">
+      <c r="E7" s="53">
         <v>5</v>
       </c>
-      <c r="F7" s="57">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="57">
+      <c r="F7" s="53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="53">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -18340,7 +18346,7 @@
       <c r="J12" s="27">
         <v>4</v>
       </c>
-      <c r="L12" s="60" t="s">
+      <c r="L12" s="55" t="s">
         <v>102</v>
       </c>
     </row>
@@ -18504,7 +18510,7 @@
         <f t="shared" si="1"/>
         <v>3.5714285714285712</v>
       </c>
-      <c r="L17" s="60" t="s">
+      <c r="L17" s="55" t="s">
         <v>101</v>
       </c>
     </row>
@@ -18631,7 +18637,7 @@
   <dimension ref="A1:AH26"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Y11" sqref="Y11"/>
+      <selection activeCell="AH14" sqref="AH14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18652,42 +18658,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="I1" s="55" t="s">
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="I1" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="55"/>
-      <c r="L1" s="56" t="s">
+      <c r="J1" s="58"/>
+      <c r="L1" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="W1" s="55" t="s">
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="W1" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
-      <c r="AD1" s="55"/>
-      <c r="AE1" s="55"/>
-      <c r="AF1" s="55"/>
-      <c r="AG1" s="55"/>
-      <c r="AH1" s="55"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
+      <c r="Z1" s="58"/>
+      <c r="AA1" s="58"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="58"/>
+      <c r="AD1" s="58"/>
+      <c r="AE1" s="58"/>
+      <c r="AF1" s="58"/>
+      <c r="AG1" s="58"/>
+      <c r="AH1" s="58"/>
     </row>
     <row r="2" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -19136,14 +19142,14 @@
       <c r="B8" s="13">
         <v>2</v>
       </c>
-      <c r="E8" s="59">
+      <c r="E8" s="54">
         <v>6</v>
       </c>
-      <c r="F8" s="59">
+      <c r="F8" s="54">
         <f t="shared" si="0"/>
         <v>-4</v>
       </c>
-      <c r="G8" s="59">
+      <c r="G8" s="54">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -19160,14 +19166,14 @@
         <v>2</v>
       </c>
       <c r="N8"/>
-      <c r="P8" s="57">
+      <c r="P8" s="53">
         <v>6</v>
       </c>
-      <c r="Q8" s="57">
+      <c r="Q8" s="53">
         <f t="shared" si="2"/>
         <v>-4</v>
       </c>
-      <c r="R8" s="57">
+      <c r="R8" s="53">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
@@ -19425,7 +19431,7 @@
       <c r="U12" s="27">
         <v>2</v>
       </c>
-      <c r="W12" s="60" t="s">
+      <c r="W12" s="55" t="s">
         <v>102</v>
       </c>
     </row>
@@ -19653,7 +19659,7 @@
         <f t="shared" si="3"/>
         <v>0.71428571428571352</v>
       </c>
-      <c r="W17" s="60" t="s">
+      <c r="W17" s="55" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add tables and API routes for bracket refunds and matches
</commit_message>
<xml_diff>
--- a/form_design/Bracket Merge.xlsx
+++ b/form_design/Bracket Merge.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects 2017\Codecademy\Portfolio\bowl_tmnts\form_design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF36E288-F3BB-41E7-9F2A-DAB41076424E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F3AB61-CA13-4F7F-88EF-1BC6FE4AF367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="28050" windowHeight="15075" firstSheet="11" activeTab="15" xr2:uid="{A2505C3C-2350-4FE2-AF4A-826C0074D70B}"/>
+    <workbookView xWindow="29265" yWindow="195" windowWidth="28050" windowHeight="15075" firstSheet="11" activeTab="15" xr2:uid="{A2505C3C-2350-4FE2-AF4A-826C0074D70B}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate Full and Bye" sheetId="13" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3018" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2898" uniqueCount="123">
   <si>
     <t>Pos</t>
   </si>
@@ -422,126 +422,6 @@
   <si>
     <t>Tom</t>
   </si>
-  <si>
-    <t>Umar</t>
-  </si>
-  <si>
-    <t>Vince</t>
-  </si>
-  <si>
-    <t>Will</t>
-  </si>
-  <si>
-    <t>Xander</t>
-  </si>
-  <si>
-    <t>Yuri</t>
-  </si>
-  <si>
-    <t>Zane</t>
-  </si>
-  <si>
-    <t>Adam</t>
-  </si>
-  <si>
-    <t>Ben</t>
-  </si>
-  <si>
-    <t>Carl</t>
-  </si>
-  <si>
-    <t>Dave</t>
-  </si>
-  <si>
-    <t>Eli</t>
-  </si>
-  <si>
-    <t>Finn</t>
-  </si>
-  <si>
-    <t>Gabe</t>
-  </si>
-  <si>
-    <t>Hank</t>
-  </si>
-  <si>
-    <t>Isaac</t>
-  </si>
-  <si>
-    <t>Kyle</t>
-  </si>
-  <si>
-    <t>Liam</t>
-  </si>
-  <si>
-    <t>Mark</t>
-  </si>
-  <si>
-    <t>Noah</t>
-  </si>
-  <si>
-    <t>Owen</t>
-  </si>
-  <si>
-    <t>Pete</t>
-  </si>
-  <si>
-    <t>Ric</t>
-  </si>
-  <si>
-    <t>Stu</t>
-  </si>
-  <si>
-    <t>Ted</t>
-  </si>
-  <si>
-    <t>Vic</t>
-  </si>
-  <si>
-    <t>Wes</t>
-  </si>
-  <si>
-    <t>Xavier</t>
-  </si>
-  <si>
-    <t>Yann</t>
-  </si>
-  <si>
-    <t>Zeke</t>
-  </si>
-  <si>
-    <t>Aaron</t>
-  </si>
-  <si>
-    <t>Bill</t>
-  </si>
-  <si>
-    <t>Cam</t>
-  </si>
-  <si>
-    <t>Dick</t>
-  </si>
-  <si>
-    <t>Eric</t>
-  </si>
-  <si>
-    <t>Felix</t>
-  </si>
-  <si>
-    <t>Gary</t>
-  </si>
-  <si>
-    <t>Harry</t>
-  </si>
-  <si>
-    <t>Ivan</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Joe</t>
-  </si>
 </sst>
 </file>
 
@@ -586,7 +466,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -713,6 +593,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB05800"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -778,7 +670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -907,36 +799,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -948,16 +827,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFB05800"/>
+      <color rgb="FFEA7500"/>
       <color rgb="FFD60000"/>
       <color rgb="FFC9C400"/>
-      <color rgb="FFEA7500"/>
       <color rgb="FFFF3300"/>
       <color rgb="FFCC9900"/>
       <color rgb="FFFF9933"/>
       <color rgb="FFFFFF66"/>
       <color rgb="FFFF9966"/>
       <color rgb="FFFF7171"/>
-      <color rgb="FFFE9898"/>
     </mruColors>
   </colors>
   <extLst>
@@ -7321,7 +7200,7 @@
       </c>
       <c r="B23" s="1">
         <f ca="1">INT((RAND()*10)+1)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="W23" t="s">
         <v>79</v>
@@ -8728,7 +8607,7 @@
       </c>
       <c r="B23" s="1">
         <f ca="1">INT((RAND()*10)+1)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="W23" t="s">
         <v>79</v>
@@ -10221,7 +10100,7 @@
       </c>
       <c r="B23" s="1">
         <f ca="1">INT((RAND()*10)+1)</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E23" s="1">
         <v>21</v>
@@ -10559,7 +10438,7 @@
     <mergeCell ref="W1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="J23">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>$I$23</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10569,10 +10448,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F623FF4-7939-4653-B0BB-94DA0D3CEA97}">
-  <dimension ref="A1:BL83"/>
+  <dimension ref="A1:BL82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10750,47 +10629,47 @@
         <v>10</v>
       </c>
       <c r="D3" s="1">
-        <f>B63</f>
-        <v>594</v>
+        <f>B23</f>
+        <v>133</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
       </c>
       <c r="F3" s="1">
         <f>($D$3-(8*E3))/7</f>
-        <v>83.714285714285708</v>
+        <v>17.857142857142858</v>
       </c>
       <c r="G3" s="1">
         <f>E3+F3</f>
-        <v>84.714285714285708</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="J3" s="63">
-        <v>100</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="M3" s="63">
-        <v>100</v>
+        <v>18.857142857142858</v>
+      </c>
+      <c r="I3" s="64" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="65">
+        <v>20</v>
+      </c>
+      <c r="L3" s="64" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="65">
+        <v>17</v>
       </c>
       <c r="N3"/>
       <c r="O3" s="1">
-        <f>M63</f>
-        <v>594</v>
+        <f>M23</f>
+        <v>130</v>
       </c>
       <c r="P3" s="1">
         <v>1</v>
       </c>
       <c r="Q3" s="1">
         <f>($O$3-(8*P3))/7</f>
-        <v>83.714285714285708</v>
+        <v>17.428571428571427</v>
       </c>
       <c r="R3" s="1">
         <f>P3+Q3</f>
-        <v>84.714285714285708</v>
+        <v>18.428571428571427</v>
       </c>
       <c r="T3" s="20" t="s">
         <v>12</v>
@@ -10832,30 +10711,30 @@
         <v>13</v>
       </c>
       <c r="B4" s="4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" ref="F4:F36" si="0">($D$3-(8*E4))/7</f>
-        <v>82.571428571428569</v>
+        <v>16.714285714285715</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" ref="G4:G36" si="1">E4+F4</f>
-        <v>84.571428571428569</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="J4" s="65">
-        <v>20</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="M4" s="65">
-        <v>20</v>
+        <v>18.714285714285715</v>
+      </c>
+      <c r="I4" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="49">
+        <v>10</v>
+      </c>
+      <c r="L4" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="49">
+        <v>10</v>
       </c>
       <c r="N4"/>
       <c r="P4" s="1">
@@ -10863,11 +10742,11 @@
       </c>
       <c r="Q4" s="1">
         <f t="shared" ref="Q4:Q34" si="2">($O$3-(8*P4))/7</f>
-        <v>82.571428571428569</v>
+        <v>16.285714285714285</v>
       </c>
       <c r="R4" s="1">
         <f t="shared" ref="R4:R34" si="3">P4+Q4</f>
-        <v>84.571428571428569</v>
+        <v>18.285714285714285</v>
       </c>
       <c r="T4" s="3" t="s">
         <v>13</v>
@@ -10909,30 +10788,30 @@
         <v>14</v>
       </c>
       <c r="B5" s="6">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E5" s="1">
         <v>3</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>81.428571428571431</v>
+        <v>15.571428571428571</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="1"/>
-        <v>84.428571428571431</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="J5" s="65">
-        <v>20</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="M5" s="65">
-        <v>20</v>
+        <v>18.571428571428569</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="23">
+        <v>9</v>
+      </c>
+      <c r="L5" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="23">
+        <v>9</v>
       </c>
       <c r="N5"/>
       <c r="P5" s="1">
@@ -10940,11 +10819,11 @@
       </c>
       <c r="Q5" s="1">
         <f t="shared" si="2"/>
-        <v>81.428571428571431</v>
+        <v>15.142857142857142</v>
       </c>
       <c r="R5" s="1">
         <f t="shared" si="3"/>
-        <v>84.428571428571431</v>
+        <v>18.142857142857142</v>
       </c>
       <c r="T5" s="5" t="s">
         <v>14</v>
@@ -10986,30 +10865,30 @@
         <v>15</v>
       </c>
       <c r="B6" s="9">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E6" s="1">
         <v>4</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>80.285714285714292</v>
+        <v>14.428571428571429</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="1"/>
-        <v>84.285714285714292</v>
-      </c>
-      <c r="I6" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="49">
-        <v>10</v>
-      </c>
-      <c r="L6" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="M6" s="49">
-        <v>10</v>
+        <v>18.428571428571431</v>
+      </c>
+      <c r="I6" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="J6" s="40">
+        <v>9</v>
+      </c>
+      <c r="L6" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="M6" s="40">
+        <v>9</v>
       </c>
       <c r="N6"/>
       <c r="P6" s="1">
@@ -11017,11 +10896,11 @@
       </c>
       <c r="Q6" s="1">
         <f t="shared" si="2"/>
-        <v>80.285714285714292</v>
+        <v>14</v>
       </c>
       <c r="R6" s="1">
         <f t="shared" si="3"/>
-        <v>84.285714285714292</v>
+        <v>18</v>
       </c>
       <c r="T6" s="8" t="s">
         <v>15</v>
@@ -11061,30 +10940,30 @@
         <v>16</v>
       </c>
       <c r="B7" s="11">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E7" s="1">
         <v>5</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>79.142857142857139</v>
+        <v>13.285714285714286</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="1"/>
-        <v>84.142857142857139</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="4">
-        <v>10</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="M7" s="4">
-        <v>10</v>
+        <v>18.285714285714285</v>
+      </c>
+      <c r="I7" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" s="44">
+        <v>9</v>
+      </c>
+      <c r="L7" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="M7" s="44">
+        <v>9</v>
       </c>
       <c r="N7"/>
       <c r="P7" s="1">
@@ -11092,11 +10971,11 @@
       </c>
       <c r="Q7" s="1">
         <f t="shared" si="2"/>
-        <v>79.142857142857139</v>
+        <v>12.857142857142858</v>
       </c>
       <c r="R7" s="1">
         <f t="shared" si="3"/>
-        <v>84.142857142857139</v>
+        <v>17.857142857142858</v>
       </c>
       <c r="T7" s="10" t="s">
         <v>16</v>
@@ -11136,30 +11015,30 @@
         <v>17</v>
       </c>
       <c r="B8" s="13">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E8" s="1">
         <v>6</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>78</v>
+        <v>12.142857142857142</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="1"/>
-        <v>84</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="6">
-        <v>10</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M8" s="6">
-        <v>10</v>
+        <v>18.142857142857142</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="4">
+        <v>8</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" s="4">
+        <v>8</v>
       </c>
       <c r="N8"/>
       <c r="P8" s="1">
@@ -11167,11 +11046,11 @@
       </c>
       <c r="Q8" s="1">
         <f t="shared" si="2"/>
-        <v>78</v>
+        <v>11.714285714285714</v>
       </c>
       <c r="R8" s="1">
         <f t="shared" si="3"/>
-        <v>84</v>
+        <v>17.714285714285715</v>
       </c>
       <c r="T8" s="12" t="s">
         <v>17</v>
@@ -11211,30 +11090,30 @@
         <v>18</v>
       </c>
       <c r="B9" s="19">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E9" s="1">
         <v>7</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
-        <v>76.857142857142861</v>
+        <v>11</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="1"/>
-        <v>83.857142857142861</v>
+        <v>18</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>15</v>
       </c>
       <c r="J9" s="9">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>15</v>
       </c>
       <c r="M9" s="9">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="N9"/>
       <c r="P9" s="1">
@@ -11242,11 +11121,11 @@
       </c>
       <c r="Q9" s="1">
         <f t="shared" si="2"/>
-        <v>76.857142857142861</v>
+        <v>10.571428571428571</v>
       </c>
       <c r="R9" s="1">
         <f t="shared" si="3"/>
-        <v>83.857142857142861</v>
+        <v>17.571428571428569</v>
       </c>
       <c r="T9" s="18" t="s">
         <v>18</v>
@@ -11286,30 +11165,30 @@
         <v>19</v>
       </c>
       <c r="B10" s="23">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1">
         <v>8</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="0"/>
-        <v>75.714285714285708</v>
+        <v>9.8571428571428577</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="1"/>
-        <v>83.714285714285708</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="11">
-        <v>10</v>
-      </c>
-      <c r="L10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="M10" s="11">
-        <v>10</v>
+        <v>17.857142857142858</v>
+      </c>
+      <c r="I10" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10" s="42">
+        <v>7</v>
+      </c>
+      <c r="L10" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="M10" s="42">
+        <v>7</v>
       </c>
       <c r="N10"/>
       <c r="P10" s="1">
@@ -11317,11 +11196,11 @@
       </c>
       <c r="Q10" s="1">
         <f t="shared" si="2"/>
-        <v>75.714285714285708</v>
+        <v>9.4285714285714288</v>
       </c>
       <c r="R10" s="1">
         <f t="shared" si="3"/>
-        <v>83.714285714285708</v>
+        <v>17.428571428571431</v>
       </c>
       <c r="T10" s="22" t="s">
         <v>19</v>
@@ -11361,30 +11240,30 @@
         <v>22</v>
       </c>
       <c r="B11" s="25">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E11" s="1">
         <v>9</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="0"/>
-        <v>74.571428571428569</v>
+        <v>8.7142857142857135</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="1"/>
-        <v>83.571428571428569</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="13">
-        <v>10</v>
-      </c>
-      <c r="L11" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="M11" s="13">
-        <v>10</v>
+        <v>17.714285714285715</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="6">
+        <v>6</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" s="6">
+        <v>6</v>
       </c>
       <c r="N11"/>
       <c r="P11" s="1">
@@ -11392,11 +11271,11 @@
       </c>
       <c r="Q11" s="1">
         <f t="shared" si="2"/>
-        <v>74.571428571428569</v>
+        <v>8.2857142857142865</v>
       </c>
       <c r="R11" s="1">
         <f t="shared" si="3"/>
-        <v>83.571428571428569</v>
+        <v>17.285714285714285</v>
       </c>
       <c r="T11" s="24" t="s">
         <v>22</v>
@@ -11410,30 +11289,30 @@
         <v>23</v>
       </c>
       <c r="B12" s="27">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E12" s="1">
         <v>10</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="0"/>
-        <v>73.428571428571431</v>
+        <v>7.5714285714285712</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="1"/>
-        <v>83.428571428571431</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" s="19">
-        <v>10</v>
-      </c>
-      <c r="L12" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="M12" s="19">
-        <v>10</v>
+        <v>17.571428571428569</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="11">
+        <v>6</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12" s="11">
+        <v>6</v>
       </c>
       <c r="N12"/>
       <c r="P12" s="1">
@@ -11441,11 +11320,11 @@
       </c>
       <c r="Q12" s="1">
         <f t="shared" si="2"/>
-        <v>73.428571428571431</v>
+        <v>7.1428571428571432</v>
       </c>
       <c r="R12" s="1">
         <f t="shared" si="3"/>
-        <v>83.428571428571431</v>
+        <v>17.142857142857142</v>
       </c>
       <c r="T12" s="26" t="s">
         <v>23</v>
@@ -11462,30 +11341,30 @@
         <v>24</v>
       </c>
       <c r="B13" s="29">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E13" s="1">
         <v>11</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="0"/>
-        <v>72.285714285714292</v>
+        <v>6.4285714285714288</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="1"/>
-        <v>83.285714285714292</v>
-      </c>
-      <c r="I13" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="23">
-        <v>10</v>
-      </c>
-      <c r="L13" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="M13" s="23">
-        <v>10</v>
+        <v>17.428571428571431</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="19">
+        <v>6</v>
+      </c>
+      <c r="L13" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="M13" s="19">
+        <v>6</v>
       </c>
       <c r="N13"/>
       <c r="P13" s="1">
@@ -11493,11 +11372,11 @@
       </c>
       <c r="Q13" s="1">
         <f t="shared" si="2"/>
-        <v>72.285714285714292</v>
+        <v>6</v>
       </c>
       <c r="R13" s="1">
         <f t="shared" si="3"/>
-        <v>83.285714285714292</v>
+        <v>17</v>
       </c>
       <c r="T13" s="32" t="s">
         <v>24</v>
@@ -11511,30 +11390,30 @@
         <v>70</v>
       </c>
       <c r="B14" s="34">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E14" s="1">
         <v>12</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
-        <v>71.142857142857139</v>
+        <v>5.2857142857142856</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="1"/>
-        <v>83.142857142857139</v>
+        <v>17.285714285714285</v>
       </c>
       <c r="I14" s="24" t="s">
         <v>22</v>
       </c>
       <c r="J14" s="25">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="L14" s="24" t="s">
         <v>22</v>
       </c>
       <c r="M14" s="25">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="N14"/>
       <c r="P14" s="1">
@@ -11542,11 +11421,11 @@
       </c>
       <c r="Q14" s="1">
         <f t="shared" si="2"/>
-        <v>71.142857142857139</v>
+        <v>4.8571428571428568</v>
       </c>
       <c r="R14" s="1">
         <f t="shared" si="3"/>
-        <v>83.142857142857139</v>
+        <v>16.857142857142858</v>
       </c>
       <c r="T14" s="33" t="s">
         <v>70</v>
@@ -11593,30 +11472,30 @@
         <v>71</v>
       </c>
       <c r="B15" s="46">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E15" s="1">
         <v>13</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>4.1428571428571432</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="1"/>
-        <v>83</v>
-      </c>
-      <c r="I15" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" s="27">
-        <v>10</v>
-      </c>
-      <c r="L15" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="M15" s="27">
-        <v>10</v>
+        <v>17.142857142857142</v>
+      </c>
+      <c r="I15" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="J15" s="46">
+        <v>6</v>
+      </c>
+      <c r="L15" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="M15" s="46">
+        <v>6</v>
       </c>
       <c r="N15"/>
       <c r="P15" s="1">
@@ -11624,11 +11503,11 @@
       </c>
       <c r="Q15" s="1">
         <f t="shared" si="2"/>
-        <v>70</v>
+        <v>3.7142857142857144</v>
       </c>
       <c r="R15" s="1">
         <f t="shared" si="3"/>
-        <v>83</v>
+        <v>16.714285714285715</v>
       </c>
       <c r="T15" s="45" t="s">
         <v>71</v>
@@ -11675,30 +11554,30 @@
         <v>72</v>
       </c>
       <c r="B16" s="40">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" s="1">
         <v>14</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="0"/>
-        <v>68.857142857142861</v>
+        <v>3</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" si="1"/>
-        <v>82.857142857142861</v>
-      </c>
-      <c r="I16" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="J16" s="29">
-        <v>10</v>
-      </c>
-      <c r="L16" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="M16" s="29">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="I16" s="60" t="s">
+        <v>121</v>
+      </c>
+      <c r="J16" s="61">
+        <v>6</v>
+      </c>
+      <c r="L16" s="60" t="s">
+        <v>121</v>
+      </c>
+      <c r="M16" s="61">
+        <v>6</v>
       </c>
       <c r="N16"/>
       <c r="P16" s="1">
@@ -11706,11 +11585,11 @@
       </c>
       <c r="Q16" s="1">
         <f t="shared" si="2"/>
-        <v>68.857142857142861</v>
+        <v>2.5714285714285716</v>
       </c>
       <c r="R16" s="1">
         <f t="shared" si="3"/>
-        <v>82.857142857142861</v>
+        <v>16.571428571428573</v>
       </c>
       <c r="T16" s="35" t="s">
         <v>72</v>
@@ -11724,30 +11603,30 @@
         <v>73</v>
       </c>
       <c r="B17" s="41">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E17" s="1">
         <v>15</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="0"/>
-        <v>67.714285714285708</v>
+        <v>1.8571428571428572</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="1"/>
-        <v>82.714285714285708</v>
-      </c>
-      <c r="I17" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="J17" s="34">
-        <v>10</v>
-      </c>
-      <c r="L17" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="M17" s="34">
-        <v>10</v>
+        <v>16.857142857142858</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="13">
+        <v>4</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M17" s="13">
+        <v>4</v>
       </c>
       <c r="N17"/>
       <c r="P17" s="1">
@@ -11755,11 +11634,11 @@
       </c>
       <c r="Q17" s="1">
         <f t="shared" si="2"/>
-        <v>67.714285714285708</v>
+        <v>1.4285714285714286</v>
       </c>
       <c r="R17" s="1">
         <f t="shared" si="3"/>
-        <v>82.714285714285708</v>
+        <v>16.428571428571427</v>
       </c>
       <c r="T17" s="36" t="s">
         <v>73</v>
@@ -11776,30 +11655,30 @@
         <v>74</v>
       </c>
       <c r="B18" s="42">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E18" s="1">
         <v>16</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="0"/>
-        <v>66.571428571428569</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" si="1"/>
-        <v>82.571428571428569</v>
-      </c>
-      <c r="I18" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="J18" s="46">
-        <v>10</v>
-      </c>
-      <c r="L18" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="M18" s="46">
-        <v>10</v>
+        <v>16.714285714285715</v>
+      </c>
+      <c r="I18" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="J18" s="43">
+        <v>4</v>
+      </c>
+      <c r="L18" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="M18" s="43">
+        <v>4</v>
       </c>
       <c r="N18"/>
       <c r="P18" s="1">
@@ -11807,11 +11686,11 @@
       </c>
       <c r="Q18" s="1">
         <f t="shared" si="2"/>
-        <v>66.571428571428569</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="R18" s="1">
         <f t="shared" si="3"/>
-        <v>82.571428571428569</v>
+        <v>16.285714285714285</v>
       </c>
       <c r="T18" s="37" t="s">
         <v>74</v>
@@ -11825,30 +11704,30 @@
         <v>75</v>
       </c>
       <c r="B19" s="43">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E19" s="1">
         <v>17</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="0"/>
-        <v>65.428571428571431</v>
+        <v>-0.42857142857142855</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="1"/>
-        <v>82.428571428571431</v>
-      </c>
-      <c r="I19" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="J19" s="40">
-        <v>10</v>
-      </c>
-      <c r="L19" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="M19" s="40">
-        <v>10</v>
+        <v>16.571428571428573</v>
+      </c>
+      <c r="I19" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="27">
+        <v>3</v>
+      </c>
+      <c r="L19" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19" s="27">
+        <v>3</v>
       </c>
       <c r="N19"/>
       <c r="P19" s="1">
@@ -11856,11 +11735,11 @@
       </c>
       <c r="Q19" s="1">
         <f t="shared" si="2"/>
-        <v>65.428571428571431</v>
+        <v>-0.8571428571428571</v>
       </c>
       <c r="R19" s="1">
         <f t="shared" si="3"/>
-        <v>82.428571428571431</v>
+        <v>16.142857142857142</v>
       </c>
       <c r="T19" s="38" t="s">
         <v>75</v>
@@ -11919,30 +11798,30 @@
         <v>76</v>
       </c>
       <c r="B20" s="44">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E20" s="1">
         <v>18</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="0"/>
-        <v>64.285714285714292</v>
+        <v>-1.5714285714285714</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="1"/>
-        <v>82.285714285714292</v>
+        <v>16.428571428571427</v>
       </c>
       <c r="I20" s="36" t="s">
         <v>73</v>
       </c>
       <c r="J20" s="41">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L20" s="36" t="s">
         <v>73</v>
       </c>
       <c r="M20" s="41">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N20"/>
       <c r="P20" s="1">
@@ -11950,11 +11829,11 @@
       </c>
       <c r="Q20" s="1">
         <f t="shared" si="2"/>
-        <v>64.285714285714292</v>
+        <v>-2</v>
       </c>
       <c r="R20" s="1">
         <f t="shared" si="3"/>
-        <v>82.285714285714292</v>
+        <v>16</v>
       </c>
       <c r="T20" s="39" t="s">
         <v>76</v>
@@ -11964,10 +11843,10 @@
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="61">
         <v>6</v>
       </c>
       <c r="E21" s="1">
@@ -11975,76 +11854,76 @@
       </c>
       <c r="F21" s="1">
         <f t="shared" si="0"/>
-        <v>63.142857142857146</v>
+        <v>-2.7142857142857144</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="1"/>
-        <v>82.142857142857139</v>
-      </c>
-      <c r="I21" s="61" t="s">
-        <v>74</v>
-      </c>
-      <c r="J21" s="66">
-        <v>10</v>
-      </c>
-      <c r="L21" s="61" t="s">
-        <v>74</v>
-      </c>
-      <c r="M21" s="66">
-        <v>10</v>
+        <v>16.285714285714285</v>
+      </c>
+      <c r="I21" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="J21" s="34">
+        <v>2</v>
+      </c>
+      <c r="L21" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="M21" s="34">
+        <v>2</v>
       </c>
       <c r="P21" s="1">
         <v>19</v>
       </c>
       <c r="Q21" s="1">
         <f t="shared" si="2"/>
-        <v>63.142857142857146</v>
+        <v>-3.1428571428571428</v>
       </c>
       <c r="R21" s="1">
         <f t="shared" si="3"/>
-        <v>82.142857142857139</v>
+        <v>15.857142857142858</v>
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="62" t="s">
         <v>122</v>
       </c>
-      <c r="B22" s="1">
-        <v>4</v>
+      <c r="B22" s="63">
+        <v>2</v>
       </c>
       <c r="E22" s="1">
         <v>20</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>-3.8571428571428572</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="1"/>
-        <v>82</v>
+        <v>16.142857142857142</v>
       </c>
       <c r="I22" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="J22" s="67">
-        <v>10</v>
+        <v>122</v>
+      </c>
+      <c r="J22" s="63">
+        <v>2</v>
       </c>
       <c r="L22" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="M22" s="67">
-        <v>10</v>
+        <v>122</v>
+      </c>
+      <c r="M22" s="63">
+        <v>2</v>
       </c>
       <c r="P22" s="1">
         <v>20</v>
       </c>
       <c r="Q22" s="1">
         <f t="shared" si="2"/>
-        <v>62</v>
+        <v>-4.2857142857142856</v>
       </c>
       <c r="R22" s="1">
         <f t="shared" si="3"/>
-        <v>82</v>
+        <v>15.714285714285715</v>
       </c>
       <c r="W22" t="s">
         <v>116</v>
@@ -12054,45 +11933,35 @@
       </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>123</v>
-      </c>
       <c r="B23" s="1">
-        <v>8</v>
+        <f>SUM(B3:B22)</f>
+        <v>133</v>
       </c>
       <c r="E23" s="1">
         <v>21</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="0"/>
-        <v>60.857142857142854</v>
+        <v>-5</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" si="1"/>
-        <v>81.857142857142861</v>
-      </c>
-      <c r="I23" s="60" t="s">
-        <v>76</v>
-      </c>
-      <c r="J23" s="64">
-        <v>10</v>
-      </c>
-      <c r="L23" s="60" t="s">
-        <v>76</v>
-      </c>
-      <c r="M23" s="64">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="M23" s="1">
+        <f>SUM(M3:M22)</f>
+        <v>130</v>
       </c>
       <c r="P23" s="1">
         <v>21</v>
       </c>
       <c r="Q23" s="1">
         <f t="shared" si="2"/>
-        <v>60.857142857142854</v>
+        <v>-5.4285714285714288</v>
       </c>
       <c r="R23" s="1">
         <f t="shared" si="3"/>
-        <v>81.857142857142861</v>
+        <v>15.571428571428571</v>
       </c>
       <c r="W23" t="s">
         <v>79</v>
@@ -12102,45 +11971,27 @@
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>124</v>
-      </c>
-      <c r="B24" s="1">
-        <v>5</v>
-      </c>
       <c r="E24" s="1">
         <v>22</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="0"/>
-        <v>59.714285714285715</v>
+        <v>-6.1428571428571432</v>
       </c>
       <c r="G24" s="1">
         <f t="shared" si="1"/>
-        <v>81.714285714285722</v>
-      </c>
-      <c r="I24" t="s">
-        <v>135</v>
-      </c>
-      <c r="J24" s="1">
-        <v>10</v>
-      </c>
-      <c r="L24" t="s">
-        <v>135</v>
-      </c>
-      <c r="M24" s="1">
-        <v>10</v>
+        <v>15.857142857142858</v>
       </c>
       <c r="P24" s="1">
         <v>22</v>
       </c>
       <c r="Q24" s="1">
         <f t="shared" si="2"/>
-        <v>59.714285714285715</v>
+        <v>-6.5714285714285712</v>
       </c>
       <c r="R24" s="1">
         <f t="shared" si="3"/>
-        <v>81.714285714285722</v>
+        <v>15.428571428571429</v>
       </c>
       <c r="W24" t="s">
         <v>48</v>
@@ -12151,1976 +12002,1314 @@
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B25" s="1">
-        <v>9</v>
+        <f ca="1">INT((RAND()*10)+1)</f>
+        <v>7</v>
       </c>
       <c r="E25" s="1">
         <v>23</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" si="0"/>
-        <v>58.571428571428569</v>
+        <v>-7.2857142857142856</v>
       </c>
       <c r="G25" s="1">
         <f t="shared" si="1"/>
-        <v>81.571428571428569</v>
-      </c>
-      <c r="I25" t="s">
-        <v>146</v>
-      </c>
-      <c r="J25" s="1">
-        <v>10</v>
-      </c>
-      <c r="L25" t="s">
-        <v>146</v>
-      </c>
-      <c r="M25" s="1">
-        <v>10</v>
+        <v>15.714285714285715</v>
       </c>
       <c r="P25" s="1">
         <v>23</v>
       </c>
       <c r="Q25" s="1">
         <f t="shared" si="2"/>
-        <v>58.571428571428569</v>
+        <v>-7.7142857142857144</v>
       </c>
       <c r="R25" s="1">
         <f t="shared" si="3"/>
-        <v>81.571428571428569</v>
+        <v>15.285714285714285</v>
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>126</v>
-      </c>
-      <c r="B26" s="1">
-        <v>7</v>
-      </c>
       <c r="E26" s="1">
         <v>24</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" si="0"/>
-        <v>57.428571428571431</v>
+        <v>-8.4285714285714288</v>
       </c>
       <c r="G26" s="1">
         <f t="shared" si="1"/>
-        <v>81.428571428571431</v>
-      </c>
-      <c r="I26" t="s">
-        <v>152</v>
-      </c>
-      <c r="J26" s="1">
-        <v>10</v>
-      </c>
-      <c r="L26" t="s">
-        <v>152</v>
-      </c>
-      <c r="M26" s="1">
-        <v>10</v>
+        <v>15.571428571428571</v>
       </c>
       <c r="P26" s="1">
         <v>24</v>
       </c>
       <c r="Q26" s="1">
         <f t="shared" si="2"/>
-        <v>57.428571428571431</v>
+        <v>-8.8571428571428577</v>
       </c>
       <c r="R26" s="1">
         <f t="shared" si="3"/>
-        <v>81.428571428571431</v>
+        <v>15.142857142857142</v>
       </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>127</v>
-      </c>
-      <c r="B27" s="1">
-        <v>6</v>
-      </c>
       <c r="E27" s="1">
         <v>25</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" si="0"/>
-        <v>56.285714285714285</v>
+        <v>-9.5714285714285712</v>
       </c>
       <c r="G27" s="1">
         <f t="shared" si="1"/>
-        <v>81.285714285714278</v>
-      </c>
-      <c r="I27" t="s">
-        <v>159</v>
-      </c>
-      <c r="J27" s="1">
-        <v>10</v>
-      </c>
-      <c r="L27" t="s">
-        <v>159</v>
-      </c>
-      <c r="M27" s="1">
-        <v>10</v>
+        <v>15.428571428571429</v>
       </c>
       <c r="P27" s="1">
         <v>25</v>
       </c>
       <c r="Q27" s="1">
         <f t="shared" si="2"/>
-        <v>56.285714285714285</v>
+        <v>-10</v>
       </c>
       <c r="R27" s="1">
         <f t="shared" si="3"/>
-        <v>81.285714285714278</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>128</v>
-      </c>
-      <c r="B28" s="1">
-        <v>8</v>
-      </c>
       <c r="E28" s="1">
         <v>26</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" si="0"/>
-        <v>55.142857142857146</v>
+        <v>-10.714285714285714</v>
       </c>
       <c r="G28" s="1">
         <f t="shared" si="1"/>
-        <v>81.142857142857139</v>
-      </c>
-      <c r="I28" t="s">
-        <v>125</v>
-      </c>
-      <c r="J28" s="1">
-        <v>9</v>
-      </c>
-      <c r="L28" t="s">
-        <v>125</v>
-      </c>
-      <c r="M28" s="1">
-        <v>9</v>
+        <v>15.285714285714286</v>
       </c>
       <c r="P28" s="1">
         <v>26</v>
       </c>
       <c r="Q28" s="1">
         <f t="shared" si="2"/>
-        <v>55.142857142857146</v>
+        <v>-11.142857142857142</v>
       </c>
       <c r="R28" s="1">
         <f t="shared" si="3"/>
-        <v>81.142857142857139</v>
+        <v>14.857142857142858</v>
       </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>129</v>
-      </c>
-      <c r="B29" s="1">
-        <v>4</v>
-      </c>
       <c r="E29" s="1">
         <v>27</v>
       </c>
       <c r="F29" s="1">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>-11.857142857142858</v>
       </c>
       <c r="G29" s="1">
         <f t="shared" si="1"/>
-        <v>81</v>
-      </c>
-      <c r="I29" t="s">
-        <v>134</v>
-      </c>
-      <c r="J29" s="1">
-        <v>9</v>
-      </c>
-      <c r="L29" t="s">
-        <v>134</v>
-      </c>
-      <c r="M29" s="1">
-        <v>9</v>
+        <v>15.142857142857142</v>
       </c>
       <c r="P29" s="1">
         <v>27</v>
       </c>
       <c r="Q29" s="1">
         <f t="shared" si="2"/>
-        <v>54</v>
+        <v>-12.285714285714286</v>
       </c>
       <c r="R29" s="1">
         <f t="shared" si="3"/>
-        <v>81</v>
+        <v>14.714285714285714</v>
       </c>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>130</v>
-      </c>
-      <c r="B30" s="1">
-        <v>5</v>
-      </c>
       <c r="E30" s="1">
         <v>28</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" si="0"/>
-        <v>52.857142857142854</v>
+        <v>-13</v>
       </c>
       <c r="G30" s="1">
         <f t="shared" si="1"/>
-        <v>80.857142857142861</v>
-      </c>
-      <c r="I30" t="s">
-        <v>137</v>
-      </c>
-      <c r="J30" s="1">
-        <v>9</v>
-      </c>
-      <c r="L30" t="s">
-        <v>137</v>
-      </c>
-      <c r="M30" s="1">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="P30" s="1">
         <v>28</v>
       </c>
       <c r="Q30" s="1">
         <f t="shared" si="2"/>
-        <v>52.857142857142854</v>
+        <v>-13.428571428571429</v>
       </c>
       <c r="R30" s="1">
         <f t="shared" si="3"/>
-        <v>80.857142857142861</v>
+        <v>14.571428571428571</v>
       </c>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>131</v>
-      </c>
-      <c r="B31" s="1">
-        <v>7</v>
-      </c>
       <c r="E31" s="1">
         <v>29</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" si="0"/>
-        <v>51.714285714285715</v>
+        <v>-14.142857142857142</v>
       </c>
       <c r="G31" s="1">
         <f t="shared" si="1"/>
-        <v>80.714285714285722</v>
-      </c>
-      <c r="I31" t="s">
-        <v>143</v>
-      </c>
-      <c r="J31" s="1">
-        <v>9</v>
-      </c>
-      <c r="L31" t="s">
-        <v>143</v>
-      </c>
-      <c r="M31" s="1">
-        <v>9</v>
+        <v>14.857142857142858</v>
       </c>
       <c r="P31" s="1">
         <v>29</v>
       </c>
       <c r="Q31" s="1">
         <f t="shared" si="2"/>
-        <v>51.714285714285715</v>
+        <v>-14.571428571428571</v>
       </c>
       <c r="R31" s="1">
         <f t="shared" si="3"/>
-        <v>80.714285714285722</v>
+        <v>14.428571428571429</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>132</v>
-      </c>
-      <c r="B32" s="1">
-        <v>6</v>
-      </c>
       <c r="E32" s="1">
         <v>30</v>
       </c>
       <c r="F32" s="1">
         <f t="shared" si="0"/>
-        <v>50.571428571428569</v>
+        <v>-15.285714285714286</v>
       </c>
       <c r="G32" s="1">
         <f t="shared" si="1"/>
-        <v>80.571428571428569</v>
-      </c>
-      <c r="I32" t="s">
-        <v>149</v>
-      </c>
-      <c r="J32" s="1">
-        <v>9</v>
-      </c>
-      <c r="L32" t="s">
-        <v>149</v>
-      </c>
-      <c r="M32" s="1">
-        <v>9</v>
+        <v>14.714285714285714</v>
       </c>
       <c r="P32" s="1">
         <v>30</v>
       </c>
       <c r="Q32" s="1">
         <f t="shared" si="2"/>
-        <v>50.571428571428569</v>
+        <v>-15.714285714285714</v>
       </c>
       <c r="R32" s="1">
         <f t="shared" si="3"/>
-        <v>80.571428571428569</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>133</v>
-      </c>
-      <c r="B33" s="1">
-        <v>8</v>
-      </c>
+        <v>14.285714285714286</v>
+      </c>
+    </row>
+    <row r="33" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E33" s="1">
         <v>31</v>
       </c>
       <c r="F33" s="1">
         <f t="shared" si="0"/>
-        <v>49.428571428571431</v>
+        <v>-16.428571428571427</v>
       </c>
       <c r="G33" s="1">
         <f t="shared" si="1"/>
-        <v>80.428571428571431</v>
-      </c>
-      <c r="I33" t="s">
-        <v>158</v>
-      </c>
-      <c r="J33" s="1">
-        <v>9</v>
-      </c>
-      <c r="L33" t="s">
-        <v>158</v>
-      </c>
-      <c r="M33" s="1">
-        <v>9</v>
+        <v>14.571428571428573</v>
       </c>
       <c r="P33" s="1">
         <v>31</v>
       </c>
       <c r="Q33" s="1">
         <f t="shared" si="2"/>
-        <v>49.428571428571431</v>
+        <v>-16.857142857142858</v>
       </c>
       <c r="R33" s="1">
         <f t="shared" si="3"/>
-        <v>80.428571428571431</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>134</v>
-      </c>
-      <c r="B34" s="1">
-        <v>9</v>
-      </c>
+        <v>14.142857142857142</v>
+      </c>
+    </row>
+    <row r="34" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E34" s="1">
         <v>32</v>
       </c>
       <c r="F34" s="1">
         <f t="shared" si="0"/>
-        <v>48.285714285714285</v>
+        <v>-17.571428571428573</v>
       </c>
       <c r="G34" s="1">
         <f t="shared" si="1"/>
-        <v>80.285714285714278</v>
-      </c>
-      <c r="I34" t="s">
-        <v>161</v>
-      </c>
-      <c r="J34" s="1">
-        <v>9</v>
-      </c>
-      <c r="L34" t="s">
-        <v>161</v>
-      </c>
-      <c r="M34" s="1">
-        <v>9</v>
+        <v>14.428571428571427</v>
       </c>
       <c r="P34" s="1">
         <v>32</v>
       </c>
       <c r="Q34" s="1">
         <f t="shared" si="2"/>
-        <v>48.285714285714285</v>
+        <v>-18</v>
       </c>
       <c r="R34" s="1">
         <f t="shared" si="3"/>
-        <v>80.285714285714278</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>135</v>
-      </c>
-      <c r="B35" s="1">
-        <v>10</v>
-      </c>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E35" s="1">
         <v>33</v>
       </c>
       <c r="F35" s="1">
         <f t="shared" si="0"/>
-        <v>47.142857142857146</v>
+        <v>-18.714285714285715</v>
       </c>
       <c r="G35" s="1">
         <f t="shared" si="1"/>
-        <v>80.142857142857139</v>
-      </c>
-      <c r="I35" t="s">
-        <v>123</v>
-      </c>
-      <c r="J35" s="1">
-        <v>8</v>
-      </c>
-      <c r="L35" t="s">
-        <v>123</v>
-      </c>
-      <c r="M35" s="1">
-        <v>8</v>
+        <v>14.285714285714285</v>
       </c>
       <c r="P35" s="1">
         <v>33</v>
       </c>
       <c r="Q35" s="1">
         <f t="shared" ref="Q35:Q77" si="5">($O$3-(8*P35))/7</f>
-        <v>47.142857142857146</v>
+        <v>-19.142857142857142</v>
       </c>
       <c r="R35" s="1">
         <f t="shared" ref="R35:R77" si="6">P35+Q35</f>
-        <v>80.142857142857139</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>136</v>
-      </c>
-      <c r="B36" s="1">
-        <v>5</v>
-      </c>
+        <v>13.857142857142858</v>
+      </c>
+    </row>
+    <row r="36" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E36" s="1">
         <v>34</v>
       </c>
       <c r="F36" s="1">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>-19.857142857142858</v>
       </c>
       <c r="G36" s="1">
         <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="I36" t="s">
-        <v>128</v>
-      </c>
-      <c r="J36" s="1">
-        <v>8</v>
-      </c>
-      <c r="L36" t="s">
-        <v>128</v>
-      </c>
-      <c r="M36" s="1">
-        <v>8</v>
+        <v>14.142857142857142</v>
       </c>
       <c r="P36" s="1">
         <v>34</v>
       </c>
       <c r="Q36" s="1">
         <f t="shared" si="5"/>
-        <v>46</v>
+        <v>-20.285714285714285</v>
       </c>
       <c r="R36" s="1">
         <f t="shared" si="6"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>137</v>
-      </c>
-      <c r="B37" s="1">
-        <v>9</v>
-      </c>
+        <v>13.714285714285715</v>
+      </c>
+    </row>
+    <row r="37" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E37" s="1">
         <v>35</v>
       </c>
       <c r="F37" s="1">
         <f t="shared" ref="F37:F65" si="7">($D$3-(8*E37))/7</f>
-        <v>44.857142857142854</v>
+        <v>-21</v>
       </c>
       <c r="G37" s="1">
         <f t="shared" ref="G37:G65" si="8">E37+F37</f>
-        <v>79.857142857142861</v>
-      </c>
-      <c r="I37" t="s">
-        <v>133</v>
-      </c>
-      <c r="J37" s="1">
-        <v>8</v>
-      </c>
-      <c r="L37" t="s">
-        <v>133</v>
-      </c>
-      <c r="M37" s="1">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="P37" s="1">
         <v>35</v>
       </c>
       <c r="Q37" s="1">
         <f t="shared" si="5"/>
-        <v>44.857142857142854</v>
+        <v>-21.428571428571427</v>
       </c>
       <c r="R37" s="1">
         <f t="shared" si="6"/>
-        <v>79.857142857142861</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>162</v>
-      </c>
-      <c r="B38" s="1">
-        <v>4</v>
-      </c>
+        <v>13.571428571428573</v>
+      </c>
+    </row>
+    <row r="38" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E38" s="1">
         <v>36</v>
       </c>
       <c r="F38" s="1">
         <f t="shared" si="7"/>
-        <v>43.714285714285715</v>
+        <v>-22.142857142857142</v>
       </c>
       <c r="G38" s="1">
         <f t="shared" si="8"/>
-        <v>79.714285714285722</v>
-      </c>
-      <c r="I38" t="s">
-        <v>138</v>
-      </c>
-      <c r="J38" s="1">
-        <v>8</v>
-      </c>
-      <c r="L38" t="s">
-        <v>138</v>
-      </c>
-      <c r="M38" s="1">
-        <v>8</v>
+        <v>13.857142857142858</v>
       </c>
       <c r="P38" s="1">
         <v>36</v>
       </c>
       <c r="Q38" s="1">
         <f t="shared" si="5"/>
-        <v>43.714285714285715</v>
+        <v>-22.571428571428573</v>
       </c>
       <c r="R38" s="1">
         <f t="shared" si="6"/>
-        <v>79.714285714285722</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>138</v>
-      </c>
-      <c r="B39" s="1">
-        <v>8</v>
-      </c>
+        <v>13.428571428571427</v>
+      </c>
+    </row>
+    <row r="39" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E39" s="1">
         <v>37</v>
       </c>
       <c r="F39" s="1">
         <f t="shared" si="7"/>
-        <v>42.571428571428569</v>
+        <v>-23.285714285714285</v>
       </c>
       <c r="G39" s="1">
         <f t="shared" si="8"/>
-        <v>79.571428571428569</v>
-      </c>
-      <c r="I39" t="s">
-        <v>144</v>
+        <v>13.714285714285715</v>
+      </c>
+      <c r="I39" s="1">
+        <v>9</v>
       </c>
       <c r="J39" s="1">
-        <v>8</v>
-      </c>
-      <c r="L39" t="s">
-        <v>144</v>
-      </c>
-      <c r="M39" s="1">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="K39">
+        <v>11</v>
       </c>
       <c r="P39" s="1">
         <v>37</v>
       </c>
       <c r="Q39" s="1">
         <f t="shared" si="5"/>
-        <v>42.571428571428569</v>
+        <v>-23.714285714285715</v>
       </c>
       <c r="R39" s="1">
         <f t="shared" si="6"/>
-        <v>79.571428571428569</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>139</v>
-      </c>
-      <c r="B40" s="1">
-        <v>6</v>
-      </c>
+        <v>13.285714285714285</v>
+      </c>
+    </row>
+    <row r="40" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E40" s="1">
         <v>38</v>
       </c>
       <c r="F40" s="1">
         <f t="shared" si="7"/>
-        <v>41.428571428571431</v>
+        <v>-24.428571428571427</v>
       </c>
       <c r="G40" s="1">
         <f t="shared" si="8"/>
-        <v>79.428571428571431</v>
-      </c>
-      <c r="I40" t="s">
-        <v>153</v>
+        <v>13.571428571428573</v>
+      </c>
+      <c r="I40" s="1">
+        <v>0</v>
       </c>
       <c r="J40" s="1">
-        <v>8</v>
-      </c>
-      <c r="L40" t="s">
-        <v>153</v>
-      </c>
-      <c r="M40" s="1">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40" s="1">
+        <v>12</v>
+      </c>
+      <c r="M40">
+        <v>13</v>
       </c>
       <c r="P40" s="1">
         <v>38</v>
       </c>
       <c r="Q40" s="1">
         <f t="shared" si="5"/>
-        <v>41.428571428571431</v>
+        <v>-24.857142857142858</v>
       </c>
       <c r="R40" s="1">
         <f t="shared" si="6"/>
-        <v>79.428571428571431</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>140</v>
-      </c>
-      <c r="B41" s="1">
-        <v>5</v>
-      </c>
+        <v>13.142857142857142</v>
+      </c>
+    </row>
+    <row r="41" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E41" s="1">
         <v>39</v>
       </c>
       <c r="F41" s="1">
         <f t="shared" si="7"/>
-        <v>40.285714285714285</v>
+        <v>-25.571428571428573</v>
       </c>
       <c r="G41" s="1">
         <f t="shared" si="8"/>
-        <v>79.285714285714278</v>
-      </c>
-      <c r="I41" t="s">
-        <v>126</v>
-      </c>
-      <c r="J41" s="1">
-        <v>7</v>
-      </c>
-      <c r="L41" t="s">
-        <v>126</v>
-      </c>
-      <c r="M41" s="1">
-        <v>7</v>
+        <v>13.428571428571427</v>
+      </c>
+      <c r="L41" s="1">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
       </c>
       <c r="P41" s="1">
         <v>39</v>
       </c>
       <c r="Q41" s="1">
         <f t="shared" si="5"/>
-        <v>40.285714285714285</v>
+        <v>-26</v>
       </c>
       <c r="R41" s="1">
         <f t="shared" si="6"/>
-        <v>79.285714285714278</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>141</v>
-      </c>
-      <c r="B42" s="1">
-        <v>4</v>
-      </c>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E42" s="1">
         <v>40</v>
       </c>
       <c r="F42" s="1">
         <f t="shared" si="7"/>
-        <v>39.142857142857146</v>
+        <v>-26.714285714285715</v>
       </c>
       <c r="G42" s="1">
         <f t="shared" si="8"/>
-        <v>79.142857142857139</v>
-      </c>
-      <c r="I42" t="s">
-        <v>131</v>
-      </c>
-      <c r="J42" s="1">
-        <v>7</v>
-      </c>
-      <c r="L42" t="s">
-        <v>131</v>
-      </c>
-      <c r="M42" s="1">
-        <v>7</v>
+        <v>13.285714285714285</v>
       </c>
       <c r="P42" s="1">
         <v>40</v>
       </c>
       <c r="Q42" s="1">
         <f t="shared" si="5"/>
-        <v>39.142857142857146</v>
+        <v>-27.142857142857142</v>
       </c>
       <c r="R42" s="1">
         <f t="shared" si="6"/>
-        <v>79.142857142857139</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>142</v>
-      </c>
-      <c r="B43" s="1">
-        <v>7</v>
-      </c>
+        <v>12.857142857142858</v>
+      </c>
+    </row>
+    <row r="43" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E43" s="1">
         <v>41</v>
       </c>
       <c r="F43" s="1">
         <f t="shared" si="7"/>
-        <v>38</v>
+        <v>-27.857142857142858</v>
       </c>
       <c r="G43" s="1">
         <f t="shared" si="8"/>
-        <v>79</v>
-      </c>
-      <c r="I43" t="s">
-        <v>142</v>
-      </c>
-      <c r="J43" s="1">
-        <v>7</v>
-      </c>
-      <c r="L43" t="s">
-        <v>142</v>
-      </c>
-      <c r="M43" s="1">
-        <v>7</v>
+        <v>13.142857142857142</v>
       </c>
       <c r="P43" s="1">
         <v>41</v>
       </c>
       <c r="Q43" s="1">
         <f t="shared" si="5"/>
-        <v>38</v>
+        <v>-28.285714285714285</v>
       </c>
       <c r="R43" s="1">
         <f t="shared" si="6"/>
-        <v>79</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>143</v>
-      </c>
-      <c r="B44" s="1">
-        <v>9</v>
-      </c>
+        <v>12.714285714285715</v>
+      </c>
+    </row>
+    <row r="44" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E44" s="1">
         <v>42</v>
       </c>
       <c r="F44" s="1">
         <f t="shared" si="7"/>
-        <v>36.857142857142854</v>
+        <v>-29</v>
       </c>
       <c r="G44" s="1">
         <f t="shared" si="8"/>
-        <v>78.857142857142861</v>
-      </c>
-      <c r="I44" t="s">
-        <v>150</v>
-      </c>
-      <c r="J44" s="1">
-        <v>7</v>
-      </c>
-      <c r="L44" t="s">
-        <v>150</v>
-      </c>
-      <c r="M44" s="1">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="P44" s="1">
         <v>42</v>
       </c>
       <c r="Q44" s="1">
         <f t="shared" si="5"/>
-        <v>36.857142857142854</v>
+        <v>-29.428571428571427</v>
       </c>
       <c r="R44" s="1">
         <f t="shared" si="6"/>
-        <v>78.857142857142861</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>144</v>
-      </c>
-      <c r="B45" s="1">
-        <v>8</v>
-      </c>
+        <v>12.571428571428573</v>
+      </c>
+    </row>
+    <row r="45" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E45" s="1">
         <v>43</v>
       </c>
       <c r="F45" s="1">
         <f t="shared" si="7"/>
-        <v>35.714285714285715</v>
+        <v>-30.142857142857142</v>
       </c>
       <c r="G45" s="1">
         <f t="shared" si="8"/>
-        <v>78.714285714285722</v>
-      </c>
-      <c r="I45" t="s">
-        <v>157</v>
-      </c>
-      <c r="J45" s="1">
-        <v>7</v>
-      </c>
-      <c r="L45" t="s">
-        <v>157</v>
-      </c>
-      <c r="M45" s="1">
-        <v>7</v>
+        <v>12.857142857142858</v>
       </c>
       <c r="P45" s="1">
         <v>43</v>
       </c>
       <c r="Q45" s="1">
         <f t="shared" si="5"/>
-        <v>35.714285714285715</v>
+        <v>-30.571428571428573</v>
       </c>
       <c r="R45" s="1">
         <f t="shared" si="6"/>
-        <v>78.714285714285722</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>145</v>
-      </c>
-      <c r="B46" s="1">
-        <v>6</v>
-      </c>
+        <v>12.428571428571427</v>
+      </c>
+    </row>
+    <row r="46" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E46" s="1">
         <v>44</v>
       </c>
       <c r="F46" s="1">
         <f t="shared" si="7"/>
-        <v>34.571428571428569</v>
+        <v>-31.285714285714285</v>
       </c>
       <c r="G46" s="1">
         <f t="shared" si="8"/>
-        <v>78.571428571428569</v>
-      </c>
-      <c r="I46" t="s">
-        <v>160</v>
-      </c>
-      <c r="J46" s="1">
-        <v>7</v>
-      </c>
-      <c r="L46" t="s">
-        <v>160</v>
-      </c>
-      <c r="M46" s="1">
-        <v>7</v>
+        <v>12.714285714285715</v>
       </c>
       <c r="P46" s="1">
         <v>44</v>
       </c>
       <c r="Q46" s="1">
         <f t="shared" si="5"/>
-        <v>34.571428571428569</v>
+        <v>-31.714285714285715</v>
       </c>
       <c r="R46" s="1">
         <f t="shared" si="6"/>
-        <v>78.571428571428569</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>146</v>
-      </c>
-      <c r="B47" s="1">
-        <v>10</v>
-      </c>
+        <v>12.285714285714285</v>
+      </c>
+    </row>
+    <row r="47" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E47" s="1">
         <v>45</v>
       </c>
       <c r="F47" s="1">
         <f t="shared" si="7"/>
-        <v>33.428571428571431</v>
+        <v>-32.428571428571431</v>
       </c>
       <c r="G47" s="1">
         <f t="shared" si="8"/>
-        <v>78.428571428571431</v>
-      </c>
-      <c r="I47" t="s">
-        <v>121</v>
-      </c>
-      <c r="J47" s="1">
-        <v>6</v>
-      </c>
-      <c r="L47" t="s">
-        <v>121</v>
-      </c>
-      <c r="M47" s="1">
-        <v>6</v>
+        <v>12.571428571428569</v>
       </c>
       <c r="P47" s="1">
         <v>45</v>
       </c>
       <c r="Q47" s="1">
         <f t="shared" si="5"/>
-        <v>33.428571428571431</v>
+        <v>-32.857142857142854</v>
       </c>
       <c r="R47" s="1">
         <f t="shared" si="6"/>
-        <v>78.428571428571431</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>147</v>
-      </c>
-      <c r="B48" s="1">
-        <v>5</v>
-      </c>
+        <v>12.142857142857146</v>
+      </c>
+    </row>
+    <row r="48" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E48" s="1">
         <v>46</v>
       </c>
       <c r="F48" s="1">
         <f t="shared" si="7"/>
-        <v>32.285714285714285</v>
+        <v>-33.571428571428569</v>
       </c>
       <c r="G48" s="1">
         <f t="shared" si="8"/>
-        <v>78.285714285714278</v>
-      </c>
-      <c r="I48" t="s">
-        <v>127</v>
-      </c>
-      <c r="J48" s="1">
-        <v>6</v>
-      </c>
-      <c r="L48" t="s">
-        <v>127</v>
-      </c>
-      <c r="M48" s="1">
-        <v>6</v>
+        <v>12.428571428571431</v>
       </c>
       <c r="P48" s="1">
         <v>46</v>
       </c>
       <c r="Q48" s="1">
         <f t="shared" si="5"/>
-        <v>32.285714285714285</v>
+        <v>-34</v>
       </c>
       <c r="R48" s="1">
         <f t="shared" si="6"/>
-        <v>78.285714285714278</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>148</v>
-      </c>
-      <c r="B49" s="1">
-        <v>4</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E49" s="1">
         <v>47</v>
       </c>
       <c r="F49" s="1">
         <f t="shared" si="7"/>
-        <v>31.142857142857142</v>
+        <v>-34.714285714285715</v>
       </c>
       <c r="G49" s="1">
         <f t="shared" si="8"/>
-        <v>78.142857142857139</v>
-      </c>
-      <c r="I49" t="s">
-        <v>132</v>
-      </c>
-      <c r="J49" s="1">
-        <v>6</v>
-      </c>
-      <c r="L49" t="s">
-        <v>132</v>
-      </c>
-      <c r="M49" s="1">
-        <v>6</v>
+        <v>12.285714285714285</v>
       </c>
       <c r="P49" s="1">
         <v>47</v>
       </c>
       <c r="Q49" s="1">
         <f t="shared" si="5"/>
-        <v>31.142857142857142</v>
+        <v>-35.142857142857146</v>
       </c>
       <c r="R49" s="1">
         <f t="shared" si="6"/>
-        <v>78.142857142857139</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>149</v>
-      </c>
-      <c r="B50" s="1">
-        <v>9</v>
-      </c>
+        <v>11.857142857142854</v>
+      </c>
+    </row>
+    <row r="50" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E50" s="1">
         <v>48</v>
       </c>
       <c r="F50" s="1">
         <f t="shared" si="7"/>
-        <v>30</v>
+        <v>-35.857142857142854</v>
       </c>
       <c r="G50" s="1">
         <f t="shared" si="8"/>
-        <v>78</v>
-      </c>
-      <c r="I50" t="s">
-        <v>139</v>
-      </c>
-      <c r="J50" s="1">
-        <v>6</v>
-      </c>
-      <c r="L50" t="s">
-        <v>139</v>
-      </c>
-      <c r="M50" s="1">
-        <v>6</v>
+        <v>12.142857142857146</v>
       </c>
       <c r="P50" s="1">
         <v>48</v>
       </c>
       <c r="Q50" s="1">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>-36.285714285714285</v>
       </c>
       <c r="R50" s="1">
         <f t="shared" si="6"/>
-        <v>78</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>150</v>
-      </c>
-      <c r="B51" s="1">
-        <v>7</v>
-      </c>
+        <v>11.714285714285715</v>
+      </c>
+    </row>
+    <row r="51" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E51" s="1">
         <v>49</v>
       </c>
       <c r="F51" s="1">
         <f t="shared" si="7"/>
-        <v>28.857142857142858</v>
+        <v>-37</v>
       </c>
       <c r="G51" s="1">
         <f t="shared" si="8"/>
-        <v>77.857142857142861</v>
-      </c>
-      <c r="I51" t="s">
-        <v>145</v>
-      </c>
-      <c r="J51" s="1">
-        <v>6</v>
-      </c>
-      <c r="L51" t="s">
-        <v>145</v>
-      </c>
-      <c r="M51" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="P51" s="1">
         <v>49</v>
       </c>
       <c r="Q51" s="1">
         <f t="shared" si="5"/>
-        <v>28.857142857142858</v>
+        <v>-37.428571428571431</v>
       </c>
       <c r="R51" s="1">
         <f t="shared" si="6"/>
-        <v>77.857142857142861</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>151</v>
-      </c>
-      <c r="B52" s="1">
-        <v>6</v>
-      </c>
+        <v>11.571428571428569</v>
+      </c>
+    </row>
+    <row r="52" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E52" s="1">
         <v>50</v>
       </c>
       <c r="F52" s="1">
         <f t="shared" si="7"/>
-        <v>27.714285714285715</v>
+        <v>-38.142857142857146</v>
       </c>
       <c r="G52" s="1">
         <f t="shared" si="8"/>
-        <v>77.714285714285722</v>
-      </c>
-      <c r="I52" t="s">
-        <v>151</v>
-      </c>
-      <c r="J52" s="1">
-        <v>6</v>
-      </c>
-      <c r="L52" t="s">
-        <v>151</v>
-      </c>
-      <c r="M52" s="1">
-        <v>6</v>
+        <v>11.857142857142854</v>
       </c>
       <c r="P52" s="1">
         <v>50</v>
       </c>
       <c r="Q52" s="1">
         <f t="shared" si="5"/>
-        <v>27.714285714285715</v>
+        <v>-38.571428571428569</v>
       </c>
       <c r="R52" s="1">
         <f t="shared" si="6"/>
-        <v>77.714285714285722</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>152</v>
-      </c>
-      <c r="B53" s="1">
-        <v>10</v>
-      </c>
+        <v>11.428571428571431</v>
+      </c>
+    </row>
+    <row r="53" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E53" s="1">
         <v>51</v>
       </c>
       <c r="F53" s="1">
         <f t="shared" si="7"/>
-        <v>26.571428571428573</v>
+        <v>-39.285714285714285</v>
       </c>
       <c r="G53" s="1">
         <f t="shared" si="8"/>
-        <v>77.571428571428569</v>
-      </c>
-      <c r="I53" t="s">
-        <v>124</v>
-      </c>
-      <c r="J53" s="1">
-        <v>5</v>
-      </c>
-      <c r="L53" t="s">
-        <v>124</v>
-      </c>
-      <c r="M53" s="1">
-        <v>5</v>
+        <v>11.714285714285715</v>
       </c>
       <c r="P53" s="1">
         <v>51</v>
       </c>
       <c r="Q53" s="1">
         <f t="shared" si="5"/>
-        <v>26.571428571428573</v>
+        <v>-39.714285714285715</v>
       </c>
       <c r="R53" s="1">
         <f t="shared" si="6"/>
-        <v>77.571428571428569</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>153</v>
-      </c>
-      <c r="B54" s="1">
-        <v>8</v>
-      </c>
+        <v>11.285714285714285</v>
+      </c>
+    </row>
+    <row r="54" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E54" s="1">
         <v>52</v>
       </c>
       <c r="F54" s="1">
         <f t="shared" si="7"/>
-        <v>25.428571428571427</v>
+        <v>-40.428571428571431</v>
       </c>
       <c r="G54" s="1">
         <f t="shared" si="8"/>
-        <v>77.428571428571431</v>
-      </c>
-      <c r="I54" t="s">
-        <v>130</v>
-      </c>
-      <c r="J54" s="1">
-        <v>5</v>
-      </c>
-      <c r="L54" t="s">
-        <v>130</v>
-      </c>
-      <c r="M54" s="1">
-        <v>5</v>
+        <v>11.571428571428569</v>
       </c>
       <c r="P54" s="1">
         <v>52</v>
       </c>
       <c r="Q54" s="1">
         <f t="shared" si="5"/>
-        <v>25.428571428571427</v>
+        <v>-40.857142857142854</v>
       </c>
       <c r="R54" s="1">
         <f t="shared" si="6"/>
-        <v>77.428571428571431</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>154</v>
-      </c>
-      <c r="B55" s="1">
-        <v>20</v>
-      </c>
+        <v>11.142857142857146</v>
+      </c>
+    </row>
+    <row r="55" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E55" s="1">
         <v>53</v>
       </c>
       <c r="F55" s="1">
         <f t="shared" si="7"/>
-        <v>24.285714285714285</v>
+        <v>-41.571428571428569</v>
       </c>
       <c r="G55" s="1">
         <f t="shared" si="8"/>
-        <v>77.285714285714278</v>
-      </c>
-      <c r="I55" t="s">
-        <v>136</v>
-      </c>
-      <c r="J55" s="1">
-        <v>5</v>
-      </c>
-      <c r="L55" t="s">
-        <v>136</v>
-      </c>
-      <c r="M55" s="1">
-        <v>5</v>
+        <v>11.428571428571431</v>
       </c>
       <c r="P55" s="1">
         <v>53</v>
       </c>
       <c r="Q55" s="1">
         <f t="shared" si="5"/>
-        <v>24.285714285714285</v>
+        <v>-42</v>
       </c>
       <c r="R55" s="1">
         <f t="shared" si="6"/>
-        <v>77.285714285714278</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>155</v>
-      </c>
-      <c r="B56" s="1">
-        <v>20</v>
-      </c>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E56" s="1">
         <v>54</v>
       </c>
       <c r="F56" s="1">
         <f t="shared" si="7"/>
-        <v>23.142857142857142</v>
+        <v>-42.714285714285715</v>
       </c>
       <c r="G56" s="1">
         <f t="shared" si="8"/>
-        <v>77.142857142857139</v>
-      </c>
-      <c r="I56" t="s">
-        <v>140</v>
-      </c>
-      <c r="J56" s="1">
-        <v>5</v>
-      </c>
-      <c r="L56" t="s">
-        <v>140</v>
-      </c>
-      <c r="M56" s="1">
-        <v>5</v>
+        <v>11.285714285714285</v>
       </c>
       <c r="P56" s="1">
         <v>54</v>
       </c>
       <c r="Q56" s="1">
         <f t="shared" si="5"/>
-        <v>23.142857142857142</v>
+        <v>-43.142857142857146</v>
       </c>
       <c r="R56" s="1">
         <f t="shared" si="6"/>
-        <v>77.142857142857139</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>156</v>
-      </c>
-      <c r="B57" s="1">
-        <v>100</v>
-      </c>
+        <v>10.857142857142854</v>
+      </c>
+    </row>
+    <row r="57" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E57" s="1">
         <v>55</v>
       </c>
       <c r="F57" s="1">
         <f t="shared" si="7"/>
-        <v>22</v>
+        <v>-43.857142857142854</v>
       </c>
       <c r="G57" s="1">
         <f t="shared" si="8"/>
-        <v>77</v>
-      </c>
-      <c r="I57" t="s">
-        <v>147</v>
-      </c>
-      <c r="J57" s="1">
-        <v>5</v>
-      </c>
-      <c r="L57" t="s">
-        <v>147</v>
-      </c>
-      <c r="M57" s="1">
-        <v>5</v>
+        <v>11.142857142857146</v>
       </c>
       <c r="P57" s="1">
         <v>55</v>
       </c>
       <c r="Q57" s="1">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>-44.285714285714285</v>
       </c>
       <c r="R57" s="1">
         <f t="shared" si="6"/>
-        <v>77</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>157</v>
-      </c>
-      <c r="B58" s="1">
-        <v>7</v>
-      </c>
+        <v>10.714285714285715</v>
+      </c>
+    </row>
+    <row r="58" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E58" s="1">
         <v>56</v>
       </c>
       <c r="F58" s="1">
         <f t="shared" si="7"/>
-        <v>20.857142857142858</v>
+        <v>-45</v>
       </c>
       <c r="G58" s="1">
         <f t="shared" si="8"/>
-        <v>76.857142857142861</v>
-      </c>
-      <c r="I58" t="s">
-        <v>122</v>
-      </c>
-      <c r="J58" s="1">
-        <v>4</v>
-      </c>
-      <c r="L58" t="s">
-        <v>122</v>
-      </c>
-      <c r="M58" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="P58" s="1">
         <v>56</v>
       </c>
       <c r="Q58" s="1">
         <f t="shared" si="5"/>
-        <v>20.857142857142858</v>
+        <v>-45.428571428571431</v>
       </c>
       <c r="R58" s="1">
         <f t="shared" si="6"/>
-        <v>76.857142857142861</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>158</v>
-      </c>
-      <c r="B59" s="1">
-        <v>9</v>
-      </c>
+        <v>10.571428571428569</v>
+      </c>
+    </row>
+    <row r="59" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E59" s="1">
         <v>57</v>
       </c>
       <c r="F59" s="1">
         <f t="shared" si="7"/>
-        <v>19.714285714285715</v>
+        <v>-46.142857142857146</v>
       </c>
       <c r="G59" s="1">
         <f t="shared" si="8"/>
-        <v>76.714285714285722</v>
-      </c>
-      <c r="I59" t="s">
-        <v>129</v>
-      </c>
-      <c r="J59" s="1">
-        <v>4</v>
-      </c>
-      <c r="L59" t="s">
-        <v>129</v>
-      </c>
-      <c r="M59" s="1">
-        <v>4</v>
+        <v>10.857142857142854</v>
       </c>
       <c r="P59" s="1">
         <v>57</v>
       </c>
       <c r="Q59" s="1">
         <f t="shared" si="5"/>
-        <v>19.714285714285715</v>
+        <v>-46.571428571428569</v>
       </c>
       <c r="R59" s="1">
         <f t="shared" si="6"/>
-        <v>76.714285714285722</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>159</v>
-      </c>
-      <c r="B60" s="1">
-        <v>10</v>
-      </c>
+        <v>10.428571428571431</v>
+      </c>
+    </row>
+    <row r="60" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E60" s="1">
         <v>58</v>
       </c>
       <c r="F60" s="1">
         <f t="shared" si="7"/>
-        <v>18.571428571428573</v>
+        <v>-47.285714285714285</v>
       </c>
       <c r="G60" s="1">
         <f t="shared" si="8"/>
-        <v>76.571428571428569</v>
-      </c>
-      <c r="I60" t="s">
-        <v>162</v>
-      </c>
-      <c r="J60" s="1">
-        <v>4</v>
-      </c>
-      <c r="L60" t="s">
-        <v>162</v>
-      </c>
-      <c r="M60" s="1">
-        <v>4</v>
+        <v>10.714285714285715</v>
       </c>
       <c r="P60" s="1">
         <v>58</v>
       </c>
       <c r="Q60" s="1">
         <f t="shared" si="5"/>
-        <v>18.571428571428573</v>
+        <v>-47.714285714285715</v>
       </c>
       <c r="R60" s="1">
         <f t="shared" si="6"/>
-        <v>76.571428571428569</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>160</v>
-      </c>
-      <c r="B61" s="1">
-        <v>7</v>
-      </c>
+        <v>10.285714285714285</v>
+      </c>
+    </row>
+    <row r="61" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E61" s="1">
         <v>59</v>
       </c>
       <c r="F61" s="1">
         <f t="shared" si="7"/>
-        <v>17.428571428571427</v>
+        <v>-48.428571428571431</v>
       </c>
       <c r="G61" s="1">
         <f t="shared" si="8"/>
-        <v>76.428571428571431</v>
-      </c>
-      <c r="I61" t="s">
-        <v>141</v>
-      </c>
-      <c r="J61" s="1">
-        <v>4</v>
-      </c>
-      <c r="L61" t="s">
-        <v>141</v>
-      </c>
-      <c r="M61" s="1">
-        <v>4</v>
+        <v>10.571428571428569</v>
       </c>
       <c r="P61" s="1">
         <v>59</v>
       </c>
       <c r="Q61" s="1">
         <f t="shared" si="5"/>
-        <v>17.428571428571427</v>
+        <v>-48.857142857142854</v>
       </c>
       <c r="R61" s="1">
         <f t="shared" si="6"/>
-        <v>76.428571428571431</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>161</v>
-      </c>
-      <c r="B62" s="1">
-        <v>9</v>
-      </c>
+        <v>10.142857142857146</v>
+      </c>
+    </row>
+    <row r="62" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E62" s="1">
         <v>60</v>
       </c>
       <c r="F62" s="1">
         <f t="shared" si="7"/>
-        <v>16.285714285714285</v>
+        <v>-49.571428571428569</v>
       </c>
       <c r="G62" s="1">
         <f t="shared" si="8"/>
-        <v>76.285714285714278</v>
-      </c>
-      <c r="I62" t="s">
-        <v>148</v>
-      </c>
-      <c r="J62" s="1">
-        <v>4</v>
-      </c>
-      <c r="L62" t="s">
-        <v>148</v>
-      </c>
-      <c r="M62" s="1">
-        <v>4</v>
+        <v>10.428571428571431</v>
       </c>
       <c r="P62" s="1">
         <v>60</v>
       </c>
       <c r="Q62" s="1">
         <f t="shared" si="5"/>
-        <v>16.285714285714285</v>
+        <v>-50</v>
       </c>
       <c r="R62" s="1">
         <f t="shared" si="6"/>
-        <v>76.285714285714278</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B63" s="1">
-        <f>SUM(B3:B62)</f>
-        <v>594</v>
-      </c>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E63" s="1">
         <v>61</v>
       </c>
       <c r="F63" s="1">
         <f t="shared" si="7"/>
-        <v>15.142857142857142</v>
+        <v>-50.714285714285715</v>
       </c>
       <c r="G63" s="1">
         <f t="shared" si="8"/>
-        <v>76.142857142857139</v>
-      </c>
-      <c r="M63" s="1">
-        <f>SUM(M3:M62)</f>
-        <v>594</v>
+        <v>10.285714285714285</v>
       </c>
       <c r="P63" s="1">
         <v>61</v>
       </c>
       <c r="Q63" s="1">
         <f t="shared" si="5"/>
-        <v>15.142857142857142</v>
+        <v>-51.142857142857146</v>
       </c>
       <c r="R63" s="1">
         <f t="shared" si="6"/>
-        <v>76.142857142857139</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+        <v>9.8571428571428541</v>
+      </c>
+    </row>
+    <row r="64" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E64" s="1">
         <v>62</v>
       </c>
       <c r="F64" s="1">
         <f t="shared" si="7"/>
-        <v>14</v>
+        <v>-51.857142857142854</v>
       </c>
       <c r="G64" s="1">
         <f t="shared" si="8"/>
-        <v>76</v>
+        <v>10.142857142857146</v>
       </c>
       <c r="P64" s="1">
         <v>62</v>
       </c>
       <c r="Q64" s="1">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>-52.285714285714285</v>
       </c>
       <c r="R64" s="1">
         <f t="shared" si="6"/>
-        <v>76</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>118</v>
-      </c>
-      <c r="B65" s="1">
-        <f ca="1">INT((RAND()*10)+1)</f>
-        <v>4</v>
-      </c>
+        <v>9.7142857142857153</v>
+      </c>
+    </row>
+    <row r="65" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E65" s="1">
         <v>63</v>
       </c>
       <c r="F65" s="1">
         <f t="shared" si="7"/>
-        <v>12.857142857142858</v>
+        <v>-53</v>
       </c>
       <c r="G65" s="1">
         <f t="shared" si="8"/>
-        <v>75.857142857142861</v>
+        <v>10</v>
       </c>
       <c r="P65" s="1">
         <v>63</v>
       </c>
       <c r="Q65" s="1">
         <f t="shared" si="5"/>
-        <v>12.857142857142858</v>
+        <v>-53.428571428571431</v>
       </c>
       <c r="R65" s="1">
         <f t="shared" si="6"/>
-        <v>75.857142857142861</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+        <v>9.5714285714285694</v>
+      </c>
+    </row>
+    <row r="66" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E66" s="1">
         <v>64</v>
       </c>
       <c r="F66" s="1">
         <f t="shared" ref="F66:F77" si="9">($D$3-(8*E66))/7</f>
-        <v>11.714285714285714</v>
+        <v>-54.142857142857146</v>
       </c>
       <c r="G66" s="1">
         <f t="shared" ref="G66:G77" si="10">E66+F66</f>
-        <v>75.714285714285708</v>
+        <v>9.8571428571428541</v>
       </c>
       <c r="P66" s="1">
         <v>64</v>
       </c>
       <c r="Q66" s="1">
         <f t="shared" si="5"/>
-        <v>11.714285714285714</v>
+        <v>-54.571428571428569</v>
       </c>
       <c r="R66" s="1">
         <f t="shared" si="6"/>
-        <v>75.714285714285708</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+        <v>9.4285714285714306</v>
+      </c>
+    </row>
+    <row r="67" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E67" s="1">
         <v>65</v>
       </c>
       <c r="F67" s="1">
         <f t="shared" si="9"/>
-        <v>10.571428571428571</v>
+        <v>-55.285714285714285</v>
       </c>
       <c r="G67" s="1">
         <f t="shared" si="10"/>
-        <v>75.571428571428569</v>
+        <v>9.7142857142857153</v>
       </c>
       <c r="P67" s="1">
         <v>65</v>
       </c>
       <c r="Q67" s="1">
         <f t="shared" si="5"/>
-        <v>10.571428571428571</v>
+        <v>-55.714285714285715</v>
       </c>
       <c r="R67" s="1">
         <f t="shared" si="6"/>
-        <v>75.571428571428569</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+        <v>9.2857142857142847</v>
+      </c>
+    </row>
+    <row r="68" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E68" s="1">
         <v>66</v>
       </c>
       <c r="F68" s="1">
         <f t="shared" si="9"/>
-        <v>9.4285714285714288</v>
+        <v>-56.428571428571431</v>
       </c>
       <c r="G68" s="1">
         <f t="shared" si="10"/>
-        <v>75.428571428571431</v>
+        <v>9.5714285714285694</v>
       </c>
       <c r="P68" s="1">
         <v>66</v>
       </c>
       <c r="Q68" s="1">
         <f t="shared" si="5"/>
-        <v>9.4285714285714288</v>
+        <v>-56.857142857142854</v>
       </c>
       <c r="R68" s="1">
         <f t="shared" si="6"/>
-        <v>75.428571428571431</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+        <v>9.1428571428571459</v>
+      </c>
+    </row>
+    <row r="69" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E69" s="1">
         <v>67</v>
       </c>
       <c r="F69" s="1">
         <f t="shared" si="9"/>
-        <v>8.2857142857142865</v>
+        <v>-57.571428571428569</v>
       </c>
       <c r="G69" s="1">
         <f t="shared" si="10"/>
-        <v>75.285714285714292</v>
+        <v>9.4285714285714306</v>
       </c>
       <c r="P69" s="1">
         <v>67</v>
       </c>
       <c r="Q69" s="1">
         <f t="shared" si="5"/>
-        <v>8.2857142857142865</v>
+        <v>-58</v>
       </c>
       <c r="R69" s="1">
         <f t="shared" si="6"/>
-        <v>75.285714285714292</v>
-      </c>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E70" s="1">
         <v>68</v>
       </c>
       <c r="F70" s="1">
         <f t="shared" si="9"/>
-        <v>7.1428571428571432</v>
+        <v>-58.714285714285715</v>
       </c>
       <c r="G70" s="1">
         <f t="shared" si="10"/>
-        <v>75.142857142857139</v>
+        <v>9.2857142857142847</v>
       </c>
       <c r="P70" s="1">
         <v>68</v>
       </c>
       <c r="Q70" s="1">
         <f t="shared" si="5"/>
-        <v>7.1428571428571432</v>
+        <v>-59.142857142857146</v>
       </c>
       <c r="R70" s="1">
         <f t="shared" si="6"/>
-        <v>75.142857142857139</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+        <v>8.8571428571428541</v>
+      </c>
+    </row>
+    <row r="71" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E71" s="1">
         <v>69</v>
       </c>
       <c r="F71" s="1">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>-59.857142857142854</v>
       </c>
       <c r="G71" s="1">
         <f t="shared" si="10"/>
-        <v>75</v>
+        <v>9.1428571428571459</v>
       </c>
       <c r="P71" s="1">
         <v>69</v>
       </c>
       <c r="Q71" s="1">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>-60.285714285714285</v>
       </c>
       <c r="R71" s="1">
         <f t="shared" si="6"/>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+        <v>8.7142857142857153</v>
+      </c>
+    </row>
+    <row r="72" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E72" s="1">
         <v>70</v>
       </c>
       <c r="F72" s="1">
         <f t="shared" si="9"/>
-        <v>4.8571428571428568</v>
+        <v>-61</v>
       </c>
       <c r="G72" s="1">
         <f t="shared" si="10"/>
-        <v>74.857142857142861</v>
+        <v>9</v>
       </c>
       <c r="P72" s="1">
         <v>70</v>
       </c>
       <c r="Q72" s="1">
         <f t="shared" si="5"/>
-        <v>4.8571428571428568</v>
+        <v>-61.428571428571431</v>
       </c>
       <c r="R72" s="1">
         <f t="shared" si="6"/>
-        <v>74.857142857142861</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+        <v>8.5714285714285694</v>
+      </c>
+    </row>
+    <row r="73" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E73" s="1">
         <v>71</v>
       </c>
       <c r="F73" s="1">
         <f t="shared" si="9"/>
-        <v>3.7142857142857144</v>
+        <v>-62.142857142857146</v>
       </c>
       <c r="G73" s="1">
         <f t="shared" si="10"/>
-        <v>74.714285714285708</v>
+        <v>8.8571428571428541</v>
       </c>
       <c r="P73" s="1">
         <v>71</v>
       </c>
       <c r="Q73" s="1">
         <f t="shared" si="5"/>
-        <v>3.7142857142857144</v>
+        <v>-62.571428571428569</v>
       </c>
       <c r="R73" s="1">
         <f t="shared" si="6"/>
-        <v>74.714285714285708</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+        <v>8.4285714285714306</v>
+      </c>
+    </row>
+    <row r="74" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E74" s="1">
         <v>72</v>
       </c>
       <c r="F74" s="1">
         <f t="shared" si="9"/>
-        <v>2.5714285714285716</v>
+        <v>-63.285714285714285</v>
       </c>
       <c r="G74" s="1">
         <f t="shared" si="10"/>
-        <v>74.571428571428569</v>
+        <v>8.7142857142857153</v>
       </c>
       <c r="P74" s="1">
         <v>72</v>
       </c>
       <c r="Q74" s="1">
         <f t="shared" si="5"/>
-        <v>2.5714285714285716</v>
+        <v>-63.714285714285715</v>
       </c>
       <c r="R74" s="1">
         <f t="shared" si="6"/>
-        <v>74.571428571428569</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+        <v>8.2857142857142847</v>
+      </c>
+    </row>
+    <row r="75" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E75" s="1">
         <v>73</v>
       </c>
       <c r="F75" s="1">
         <f t="shared" si="9"/>
-        <v>1.4285714285714286</v>
+        <v>-64.428571428571431</v>
       </c>
       <c r="G75" s="1">
         <f t="shared" si="10"/>
-        <v>74.428571428571431</v>
+        <v>8.5714285714285694</v>
       </c>
       <c r="P75" s="1">
         <v>73</v>
       </c>
       <c r="Q75" s="1">
         <f t="shared" si="5"/>
-        <v>1.4285714285714286</v>
+        <v>-64.857142857142861</v>
       </c>
       <c r="R75" s="1">
         <f t="shared" si="6"/>
-        <v>74.428571428571431</v>
-      </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+        <v>8.1428571428571388</v>
+      </c>
+    </row>
+    <row r="76" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E76" s="1">
         <v>74</v>
       </c>
       <c r="F76" s="1">
         <f t="shared" si="9"/>
-        <v>0.2857142857142857</v>
+        <v>-65.571428571428569</v>
       </c>
       <c r="G76" s="1">
         <f t="shared" si="10"/>
-        <v>74.285714285714292</v>
+        <v>8.4285714285714306</v>
       </c>
       <c r="P76" s="1">
         <v>74</v>
       </c>
       <c r="Q76" s="1">
         <f t="shared" si="5"/>
-        <v>0.2857142857142857</v>
+        <v>-66</v>
       </c>
       <c r="R76" s="1">
         <f t="shared" si="6"/>
-        <v>74.285714285714292</v>
-      </c>
-    </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E77" s="1">
         <v>75</v>
       </c>
       <c r="F77" s="1">
         <f t="shared" si="9"/>
-        <v>-0.8571428571428571</v>
+        <v>-66.714285714285708</v>
       </c>
       <c r="G77" s="1">
         <f t="shared" si="10"/>
-        <v>74.142857142857139</v>
+        <v>8.2857142857142918</v>
       </c>
       <c r="P77" s="1">
         <v>75</v>
       </c>
       <c r="Q77" s="1">
         <f t="shared" si="5"/>
-        <v>-0.8571428571428571</v>
+        <v>-67.142857142857139</v>
       </c>
       <c r="R77" s="1">
         <f t="shared" si="6"/>
-        <v>74.142857142857139</v>
-      </c>
-    </row>
-    <row r="81" spans="1:64" x14ac:dyDescent="0.25">
+        <v>7.8571428571428612</v>
+      </c>
+    </row>
+    <row r="81" spans="3:64" x14ac:dyDescent="0.25">
       <c r="C81">
         <v>3</v>
       </c>
@@ -14139,15 +13328,6 @@
       <c r="H81">
         <v>8</v>
       </c>
-      <c r="I81" s="1">
-        <v>9</v>
-      </c>
-      <c r="J81" s="1">
-        <v>10</v>
-      </c>
-      <c r="K81">
-        <v>11</v>
-      </c>
       <c r="N81" s="1">
         <v>14</v>
       </c>
@@ -14302,13 +13482,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="82" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>1</v>
-      </c>
-      <c r="B82" s="1">
-        <v>2</v>
-      </c>
+    <row r="82" spans="3:64" x14ac:dyDescent="0.25">
       <c r="C82">
         <v>0</v>
       </c>
@@ -14327,21 +13501,6 @@
       <c r="H82">
         <v>0</v>
       </c>
-      <c r="I82" s="1">
-        <v>0</v>
-      </c>
-      <c r="J82" s="1">
-        <v>0</v>
-      </c>
-      <c r="K82">
-        <v>0</v>
-      </c>
-      <c r="L82" s="1">
-        <v>12</v>
-      </c>
-      <c r="M82">
-        <v>13</v>
-      </c>
       <c r="N82" s="1">
         <v>0</v>
       </c>
@@ -14496,23 +13655,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>0</v>
-      </c>
-      <c r="B83" s="1">
-        <v>0</v>
-      </c>
-      <c r="L83" s="1">
-        <v>0</v>
-      </c>
-      <c r="M83">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I3:J62">
-    <sortCondition descending="1" ref="J3:J62"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I3:J22">
+    <sortCondition descending="1" ref="J3:J22"/>
   </sortState>
   <mergeCells count="4">
     <mergeCell ref="D1:G1"/>

</xml_diff>

<commit_message>
Got save tmntFullData and slice working
</commit_message>
<xml_diff>
--- a/form_design/Bracket Merge.xlsx
+++ b/form_design/Bracket Merge.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects 2017\Codecademy\Portfolio\bowl_tmnts\form_design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E28C65-0C81-4E34-9BC8-AA96278AE977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C763D821-BF4F-46B6-8557-F5448A162B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="16" activeTab="20" xr2:uid="{A2505C3C-2350-4FE2-AF4A-826C0074D70B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="17" activeTab="22" xr2:uid="{A2505C3C-2350-4FE2-AF4A-826C0074D70B}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate Full and Bye" sheetId="13" r:id="rId1"/>
@@ -35,6 +35,7 @@
     <sheet name="Whole Tmnt - Vic 4" sheetId="33" r:id="rId20"/>
     <sheet name="Whole Tmnt - Vic 5" sheetId="36" r:id="rId21"/>
     <sheet name="Whole Tmnt - Vic 6" sheetId="34" r:id="rId22"/>
+    <sheet name="Whole Tmnt - Vic__" sheetId="37" r:id="rId23"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3651" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3799" uniqueCount="124">
   <si>
     <t>Pos</t>
   </si>
@@ -7228,7 +7229,7 @@
       </c>
       <c r="B23" s="1">
         <f ca="1">INT((RAND()*10)+1)</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="W23" t="s">
         <v>79</v>
@@ -8635,7 +8636,7 @@
       </c>
       <c r="B23" s="1">
         <f ca="1">INT((RAND()*10)+1)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="W23" t="s">
         <v>79</v>
@@ -10128,7 +10129,7 @@
       </c>
       <c r="B23" s="1">
         <f ca="1">INT((RAND()*10)+1)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E23" s="1">
         <v>21</v>
@@ -12076,7 +12077,7 @@
       </c>
       <c r="B26" s="1">
         <f ca="1">INT((RAND()*10)+1)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E26" s="1">
         <v>24</v>
@@ -16871,7 +16872,7 @@
       </c>
       <c r="B26" s="1">
         <f ca="1">INT((RAND()*10)+1)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E26" s="1">
         <v>24</v>
@@ -20112,7 +20113,7 @@
       </c>
       <c r="B26" s="1">
         <f ca="1">INT((RAND()*10)+1)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E26" s="1">
         <v>24</v>
@@ -24278,7 +24279,7 @@
       </c>
       <c r="B26" s="1">
         <f ca="1">INT((RAND()*10)+1)</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E26" s="1">
         <v>24</v>
@@ -25918,7 +25919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED1D9A0-0D91-4846-A978-9C20C5C75D27}">
   <dimension ref="A1:BL82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
@@ -27516,7 +27517,7 @@
       </c>
       <c r="B26" s="1">
         <f ca="1">INT((RAND()*10)+1)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E26" s="1">
         <v>24</v>
@@ -30757,7 +30758,7 @@
       </c>
       <c r="B26" s="1">
         <f ca="1">INT((RAND()*10)+1)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E26" s="1">
         <v>24</v>
@@ -32385,6 +32386,3235 @@
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I3:J23">
     <sortCondition descending="1" ref="J3:J23"/>
+  </sortState>
+  <mergeCells count="4">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="L1:U1"/>
+    <mergeCell ref="W1:AH1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26DD9DFF-427A-4E41-998B-75768492A429}">
+  <dimension ref="A1:BL82"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="7" width="9.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="10" width="9.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" customWidth="1"/>
+    <col min="12" max="13" width="9.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="4.7109375" style="1" customWidth="1"/>
+    <col min="15" max="18" width="9.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="4.7109375" customWidth="1"/>
+    <col min="20" max="21" width="9.28515625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="4.7109375" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" customWidth="1"/>
+    <col min="55" max="55" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="I1" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" s="68"/>
+      <c r="L1" s="69" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
+      <c r="S1" s="69"/>
+      <c r="T1" s="69"/>
+      <c r="U1" s="69"/>
+      <c r="W1" s="68" t="s">
+        <v>95</v>
+      </c>
+      <c r="X1" s="68"/>
+      <c r="Y1" s="68"/>
+      <c r="Z1" s="68"/>
+      <c r="AA1" s="68"/>
+      <c r="AB1" s="68"/>
+      <c r="AC1" s="68"/>
+      <c r="AD1" s="68"/>
+      <c r="AE1" s="68"/>
+      <c r="AF1" s="68"/>
+      <c r="AG1" s="68"/>
+      <c r="AH1" s="68"/>
+    </row>
+    <row r="2" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2"/>
+      <c r="O2" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="T2" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="W2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="X2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB2" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF2" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH2" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI2" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ2" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK2" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="AL2" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM2" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN2" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="AO2" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="AP2" s="17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="21">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1">
+        <f>B24</f>
+        <v>134</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <f>($D$3-(8*E3))/7</f>
+        <v>18</v>
+      </c>
+      <c r="G3" s="1">
+        <f>E3+F3</f>
+        <v>19</v>
+      </c>
+      <c r="I3" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="61">
+        <v>21</v>
+      </c>
+      <c r="L3" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="61">
+        <v>17</v>
+      </c>
+      <c r="N3"/>
+      <c r="O3" s="1">
+        <f>M24</f>
+        <v>130</v>
+      </c>
+      <c r="P3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1">
+        <f>($O$3-(8*P3))/7</f>
+        <v>17.428571428571427</v>
+      </c>
+      <c r="R3" s="1">
+        <f>P3+Q3</f>
+        <v>18.428571428571427</v>
+      </c>
+      <c r="T3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="U3" s="21">
+        <v>50</v>
+      </c>
+      <c r="W3" s="15">
+        <v>1</v>
+      </c>
+      <c r="X3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z3" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:F67" si="0">($D$3-(8*E4))/7</f>
+        <v>16.857142857142858</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" ref="G4:G67" si="1">E4+F4</f>
+        <v>18.857142857142858</v>
+      </c>
+      <c r="I4" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="49">
+        <v>10</v>
+      </c>
+      <c r="L4" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="49">
+        <v>10</v>
+      </c>
+      <c r="N4"/>
+      <c r="P4" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="1">
+        <f t="shared" ref="Q4:Q67" si="2">($O$3-(8*P4))/7</f>
+        <v>16.285714285714285</v>
+      </c>
+      <c r="R4" s="1">
+        <f t="shared" ref="R4:R67" si="3">P4+Q4</f>
+        <v>18.285714285714285</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="U4" s="4">
+        <v>1</v>
+      </c>
+      <c r="W4" s="16">
+        <v>2</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z4" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2"/>
+      <c r="AO4" s="2"/>
+      <c r="AP4" s="2"/>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="6">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>15.714285714285714</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="1"/>
+        <v>18.714285714285715</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="23">
+        <v>9</v>
+      </c>
+      <c r="L5" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="23">
+        <v>9</v>
+      </c>
+      <c r="N5"/>
+      <c r="P5" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="1">
+        <f t="shared" si="2"/>
+        <v>15.142857142857142</v>
+      </c>
+      <c r="R5" s="1">
+        <f t="shared" si="3"/>
+        <v>18.142857142857142</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="U5" s="6">
+        <v>1</v>
+      </c>
+      <c r="W5" s="16">
+        <v>3</v>
+      </c>
+      <c r="X5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z5" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="2"/>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="2"/>
+      <c r="AN5" s="2"/>
+      <c r="AO5" s="2"/>
+      <c r="AP5" s="2"/>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="9">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>14.571428571428571</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="1"/>
+        <v>18.571428571428569</v>
+      </c>
+      <c r="I6" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="J6" s="40">
+        <v>9</v>
+      </c>
+      <c r="L6" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="M6" s="40">
+        <v>9</v>
+      </c>
+      <c r="N6"/>
+      <c r="P6" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="1">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="R6" s="1">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="T6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="U6" s="9">
+        <v>1</v>
+      </c>
+      <c r="W6" s="16">
+        <v>4</v>
+      </c>
+      <c r="X6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y6" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="2"/>
+      <c r="AN6" s="2"/>
+      <c r="AO6" s="2"/>
+      <c r="AP6" s="2"/>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="11">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>13.428571428571429</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="1"/>
+        <v>18.428571428571431</v>
+      </c>
+      <c r="I7" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" s="44">
+        <v>9</v>
+      </c>
+      <c r="L7" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="M7" s="44">
+        <v>9</v>
+      </c>
+      <c r="N7"/>
+      <c r="P7" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="1">
+        <f t="shared" si="2"/>
+        <v>12.857142857142858</v>
+      </c>
+      <c r="R7" s="1">
+        <f t="shared" si="3"/>
+        <v>17.857142857142858</v>
+      </c>
+      <c r="T7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="U7" s="11">
+        <v>1</v>
+      </c>
+      <c r="W7" s="16">
+        <v>5</v>
+      </c>
+      <c r="X7" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y7" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
+      <c r="AK7" s="2"/>
+      <c r="AL7" s="2"/>
+      <c r="AM7" s="2"/>
+      <c r="AN7" s="2"/>
+      <c r="AO7" s="2"/>
+      <c r="AP7" s="2"/>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="13">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>12.285714285714286</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="1"/>
+        <v>18.285714285714285</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="4">
+        <v>8</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" s="4">
+        <v>8</v>
+      </c>
+      <c r="N8"/>
+      <c r="P8" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="1">
+        <f t="shared" si="2"/>
+        <v>11.714285714285714</v>
+      </c>
+      <c r="R8" s="1">
+        <f t="shared" si="3"/>
+        <v>17.714285714285715</v>
+      </c>
+      <c r="T8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="U8" s="13">
+        <v>1</v>
+      </c>
+      <c r="W8" s="16">
+        <v>6</v>
+      </c>
+      <c r="X8" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y8" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="2"/>
+      <c r="AK8" s="2"/>
+      <c r="AL8" s="2"/>
+      <c r="AM8" s="2"/>
+      <c r="AN8" s="2"/>
+      <c r="AO8" s="2"/>
+      <c r="AP8" s="2"/>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="19">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>11.142857142857142</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="1"/>
+        <v>18.142857142857142</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="9">
+        <v>7</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" s="9">
+        <v>7</v>
+      </c>
+      <c r="N9"/>
+      <c r="P9" s="1">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="1">
+        <f t="shared" si="2"/>
+        <v>10.571428571428571</v>
+      </c>
+      <c r="R9" s="1">
+        <f t="shared" si="3"/>
+        <v>17.571428571428569</v>
+      </c>
+      <c r="T9" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="U9" s="19">
+        <v>1</v>
+      </c>
+      <c r="W9" s="16">
+        <v>7</v>
+      </c>
+      <c r="X9" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y9" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2"/>
+      <c r="AJ9" s="2"/>
+      <c r="AK9" s="2"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="2"/>
+      <c r="AN9" s="2"/>
+      <c r="AO9" s="2"/>
+      <c r="AP9" s="2"/>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="23">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="I10" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10" s="42">
+        <v>7</v>
+      </c>
+      <c r="L10" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="M10" s="42">
+        <v>7</v>
+      </c>
+      <c r="N10"/>
+      <c r="P10" s="1">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="1">
+        <f t="shared" si="2"/>
+        <v>9.4285714285714288</v>
+      </c>
+      <c r="R10" s="1">
+        <f t="shared" si="3"/>
+        <v>17.428571428571431</v>
+      </c>
+      <c r="T10" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="U10" s="23">
+        <v>1</v>
+      </c>
+      <c r="W10" s="16">
+        <v>8</v>
+      </c>
+      <c r="X10" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y10" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="2"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="2"/>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="2"/>
+      <c r="AJ10" s="2"/>
+      <c r="AK10" s="2"/>
+      <c r="AL10" s="2"/>
+      <c r="AM10" s="2"/>
+      <c r="AN10" s="2"/>
+      <c r="AO10" s="2"/>
+      <c r="AP10" s="2"/>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="25">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1">
+        <v>9</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>8.8571428571428577</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="1"/>
+        <v>17.857142857142858</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="6">
+        <v>6</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" s="6">
+        <v>6</v>
+      </c>
+      <c r="N11"/>
+      <c r="P11" s="1">
+        <v>9</v>
+      </c>
+      <c r="Q11" s="1">
+        <f t="shared" si="2"/>
+        <v>8.2857142857142865</v>
+      </c>
+      <c r="R11" s="1">
+        <f t="shared" si="3"/>
+        <v>17.285714285714285</v>
+      </c>
+      <c r="T11" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="U11" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="27">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="0"/>
+        <v>7.7142857142857144</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="1"/>
+        <v>17.714285714285715</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="11">
+        <v>6</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12" s="11">
+        <v>6</v>
+      </c>
+      <c r="N12"/>
+      <c r="P12" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q12" s="1">
+        <f t="shared" si="2"/>
+        <v>7.1428571428571432</v>
+      </c>
+      <c r="R12" s="1">
+        <f t="shared" si="3"/>
+        <v>17.142857142857142</v>
+      </c>
+      <c r="T12" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="U12" s="27">
+        <v>1</v>
+      </c>
+      <c r="W12" s="55" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="29">
+        <v>21</v>
+      </c>
+      <c r="E13" s="1">
+        <v>11</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="0"/>
+        <v>6.5714285714285712</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="1"/>
+        <v>17.571428571428569</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="19">
+        <v>6</v>
+      </c>
+      <c r="L13" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="M13" s="19">
+        <v>6</v>
+      </c>
+      <c r="N13"/>
+      <c r="P13" s="1">
+        <v>11</v>
+      </c>
+      <c r="Q13" s="1">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="R13" s="1">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="T13" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="U13" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="34">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>12</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="0"/>
+        <v>5.4285714285714288</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="1"/>
+        <v>17.428571428571431</v>
+      </c>
+      <c r="I14" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="25">
+        <v>6</v>
+      </c>
+      <c r="L14" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" s="25">
+        <v>6</v>
+      </c>
+      <c r="N14"/>
+      <c r="P14" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q14" s="1">
+        <f t="shared" si="2"/>
+        <v>4.8571428571428568</v>
+      </c>
+      <c r="R14" s="1">
+        <f t="shared" si="3"/>
+        <v>16.857142857142858</v>
+      </c>
+      <c r="T14" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="U14" s="34">
+        <v>1</v>
+      </c>
+      <c r="W14" t="s">
+        <v>77</v>
+      </c>
+      <c r="X14" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="16">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="16">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="16">
+        <v>1</v>
+      </c>
+      <c r="AD14" s="16">
+        <v>8</v>
+      </c>
+      <c r="AE14" s="16">
+        <v>8</v>
+      </c>
+      <c r="AF14" s="16">
+        <v>8</v>
+      </c>
+      <c r="AG14" s="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A15" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="46">
+        <v>6</v>
+      </c>
+      <c r="E15" s="1">
+        <v>13</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="0"/>
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="1"/>
+        <v>17.285714285714285</v>
+      </c>
+      <c r="I15" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="J15" s="46">
+        <v>6</v>
+      </c>
+      <c r="L15" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="M15" s="46">
+        <v>6</v>
+      </c>
+      <c r="N15"/>
+      <c r="P15" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q15" s="1">
+        <f t="shared" si="2"/>
+        <v>3.7142857142857144</v>
+      </c>
+      <c r="R15" s="1">
+        <f t="shared" si="3"/>
+        <v>16.714285714285715</v>
+      </c>
+      <c r="T15" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="U15" s="46">
+        <v>1</v>
+      </c>
+      <c r="W15" t="s">
+        <v>78</v>
+      </c>
+      <c r="X15" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="16">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="16">
+        <v>7</v>
+      </c>
+      <c r="AE15" s="16">
+        <v>7</v>
+      </c>
+      <c r="AF15" s="16">
+        <v>7</v>
+      </c>
+      <c r="AG15" s="16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A16" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="40">
+        <v>9</v>
+      </c>
+      <c r="E16" s="1">
+        <v>14</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="0"/>
+        <v>3.1428571428571428</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="1"/>
+        <v>17.142857142857142</v>
+      </c>
+      <c r="I16" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="J16" s="57">
+        <v>6</v>
+      </c>
+      <c r="L16" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="M16" s="57">
+        <v>6</v>
+      </c>
+      <c r="N16"/>
+      <c r="P16" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q16" s="1">
+        <f t="shared" si="2"/>
+        <v>2.5714285714285716</v>
+      </c>
+      <c r="R16" s="1">
+        <f t="shared" si="3"/>
+        <v>16.571428571428573</v>
+      </c>
+      <c r="T16" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="U16" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A17" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="41">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1">
+        <v>15</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="13">
+        <v>4</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M17" s="13">
+        <v>4</v>
+      </c>
+      <c r="N17"/>
+      <c r="P17" s="1">
+        <v>15</v>
+      </c>
+      <c r="Q17" s="1">
+        <f t="shared" si="2"/>
+        <v>1.4285714285714286</v>
+      </c>
+      <c r="R17" s="1">
+        <f t="shared" si="3"/>
+        <v>16.428571428571427</v>
+      </c>
+      <c r="T17" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="U17" s="41">
+        <v>1</v>
+      </c>
+      <c r="W17" s="55" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A18" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="42">
+        <v>7</v>
+      </c>
+      <c r="E18" s="1">
+        <v>16</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="1"/>
+        <v>16.857142857142858</v>
+      </c>
+      <c r="I18" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="J18" s="43">
+        <v>4</v>
+      </c>
+      <c r="L18" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="M18" s="43">
+        <v>4</v>
+      </c>
+      <c r="N18"/>
+      <c r="P18" s="1">
+        <v>16</v>
+      </c>
+      <c r="Q18" s="1">
+        <f t="shared" si="2"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="R18" s="1">
+        <f t="shared" si="3"/>
+        <v>16.285714285714285</v>
+      </c>
+      <c r="T18" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="U18" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A19" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="43">
+        <v>4</v>
+      </c>
+      <c r="E19" s="1">
+        <v>17</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.2857142857142857</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="1"/>
+        <v>16.714285714285715</v>
+      </c>
+      <c r="I19" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="27">
+        <v>3</v>
+      </c>
+      <c r="L19" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19" s="27">
+        <v>3</v>
+      </c>
+      <c r="N19"/>
+      <c r="P19" s="1">
+        <v>17</v>
+      </c>
+      <c r="Q19" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.8571428571428571</v>
+      </c>
+      <c r="R19" s="1">
+        <f t="shared" si="3"/>
+        <v>16.142857142857142</v>
+      </c>
+      <c r="T19" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="U19" s="43">
+        <v>1</v>
+      </c>
+      <c r="W19" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="X19" s="16">
+        <f t="shared" ref="X19:AE19" si="4">Y19-1</f>
+        <v>1</v>
+      </c>
+      <c r="Y19" s="16">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="Z19" s="16">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="AA19" s="16">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="AB19" s="16">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="AC19" s="16">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="AD19" s="16">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="AE19" s="16">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="AF19" s="16">
+        <f>AG19-1</f>
+        <v>9</v>
+      </c>
+      <c r="AG19" s="16">
+        <v>10</v>
+      </c>
+      <c r="AH19" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A20" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="44">
+        <v>9</v>
+      </c>
+      <c r="E20" s="1">
+        <v>18</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.4285714285714286</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="1"/>
+        <v>16.571428571428573</v>
+      </c>
+      <c r="I20" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="J20" s="41">
+        <v>3</v>
+      </c>
+      <c r="L20" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="M20" s="41">
+        <v>3</v>
+      </c>
+      <c r="N20"/>
+      <c r="P20" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q20" s="1">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="R20" s="1">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="T20" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="U20" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A21" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" s="57">
+        <v>6</v>
+      </c>
+      <c r="E21" s="1">
+        <v>19</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="0"/>
+        <v>-2.5714285714285716</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="1"/>
+        <v>16.428571428571427</v>
+      </c>
+      <c r="I21" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="J21" s="34">
+        <v>2</v>
+      </c>
+      <c r="L21" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="M21" s="34">
+        <v>2</v>
+      </c>
+      <c r="P21" s="1">
+        <v>19</v>
+      </c>
+      <c r="Q21" s="1">
+        <f t="shared" si="2"/>
+        <v>-3.1428571428571428</v>
+      </c>
+      <c r="R21" s="1">
+        <f t="shared" si="3"/>
+        <v>15.857142857142858</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A22" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" s="63">
+        <v>2</v>
+      </c>
+      <c r="E22" s="1">
+        <v>20</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="0"/>
+        <v>-3.7142857142857144</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="1"/>
+        <v>16.285714285714285</v>
+      </c>
+      <c r="I22" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="J22" s="63">
+        <v>2</v>
+      </c>
+      <c r="L22" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="M22" s="63">
+        <v>2</v>
+      </c>
+      <c r="P22" s="1">
+        <v>20</v>
+      </c>
+      <c r="Q22" s="1">
+        <f t="shared" si="2"/>
+        <v>-4.2857142857142856</v>
+      </c>
+      <c r="R22" s="1">
+        <f t="shared" si="3"/>
+        <v>15.714285714285715</v>
+      </c>
+      <c r="W22" t="s">
+        <v>116</v>
+      </c>
+      <c r="X22">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A23" s="64" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" s="65">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>21</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="0"/>
+        <v>-4.8571428571428568</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="1"/>
+        <v>16.142857142857142</v>
+      </c>
+      <c r="P23" s="1">
+        <v>21</v>
+      </c>
+      <c r="Q23" s="1">
+        <f t="shared" si="2"/>
+        <v>-5.4285714285714288</v>
+      </c>
+      <c r="R23" s="1">
+        <f t="shared" si="3"/>
+        <v>15.571428571428571</v>
+      </c>
+      <c r="W23" t="s">
+        <v>79</v>
+      </c>
+      <c r="X23">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <f>SUM(B3:B23)</f>
+        <v>134</v>
+      </c>
+      <c r="E24" s="1">
+        <v>22</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="M24" s="1">
+        <f>SUM(M3:M23)</f>
+        <v>130</v>
+      </c>
+      <c r="P24" s="1">
+        <v>22</v>
+      </c>
+      <c r="Q24" s="1">
+        <f t="shared" si="2"/>
+        <v>-6.5714285714285712</v>
+      </c>
+      <c r="R24" s="1">
+        <f t="shared" si="3"/>
+        <v>15.428571428571429</v>
+      </c>
+      <c r="W24" t="s">
+        <v>48</v>
+      </c>
+      <c r="X24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="E25" s="1">
+        <v>23</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="0"/>
+        <v>-7.1428571428571432</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="1"/>
+        <v>15.857142857142858</v>
+      </c>
+      <c r="P25" s="1">
+        <v>23</v>
+      </c>
+      <c r="Q25" s="1">
+        <f t="shared" si="2"/>
+        <v>-7.7142857142857144</v>
+      </c>
+      <c r="R25" s="1">
+        <f t="shared" si="3"/>
+        <v>15.285714285714285</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" s="1">
+        <f ca="1">INT((RAND()*10)+1)</f>
+        <v>6</v>
+      </c>
+      <c r="E26" s="1">
+        <v>24</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="0"/>
+        <v>-8.2857142857142865</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="1"/>
+        <v>15.714285714285714</v>
+      </c>
+      <c r="P26" s="1">
+        <v>24</v>
+      </c>
+      <c r="Q26" s="1">
+        <f t="shared" si="2"/>
+        <v>-8.8571428571428577</v>
+      </c>
+      <c r="R26" s="1">
+        <f t="shared" si="3"/>
+        <v>15.142857142857142</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="E27" s="1">
+        <v>25</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="0"/>
+        <v>-9.4285714285714288</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" si="1"/>
+        <v>15.571428571428571</v>
+      </c>
+      <c r="P27" s="1">
+        <v>25</v>
+      </c>
+      <c r="Q27" s="1">
+        <f t="shared" si="2"/>
+        <v>-10</v>
+      </c>
+      <c r="R27" s="1">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="E28" s="1">
+        <v>26</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="0"/>
+        <v>-10.571428571428571</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" si="1"/>
+        <v>15.428571428571429</v>
+      </c>
+      <c r="P28" s="1">
+        <v>26</v>
+      </c>
+      <c r="Q28" s="1">
+        <f t="shared" si="2"/>
+        <v>-11.142857142857142</v>
+      </c>
+      <c r="R28" s="1">
+        <f t="shared" si="3"/>
+        <v>14.857142857142858</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="E29" s="1">
+        <v>27</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="0"/>
+        <v>-11.714285714285714</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="1"/>
+        <v>15.285714285714286</v>
+      </c>
+      <c r="P29" s="1">
+        <v>27</v>
+      </c>
+      <c r="Q29" s="1">
+        <f t="shared" si="2"/>
+        <v>-12.285714285714286</v>
+      </c>
+      <c r="R29" s="1">
+        <f t="shared" si="3"/>
+        <v>14.714285714285714</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="E30" s="1">
+        <v>28</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="0"/>
+        <v>-12.857142857142858</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="1"/>
+        <v>15.142857142857142</v>
+      </c>
+      <c r="P30" s="1">
+        <v>28</v>
+      </c>
+      <c r="Q30" s="1">
+        <f t="shared" si="2"/>
+        <v>-13.428571428571429</v>
+      </c>
+      <c r="R30" s="1">
+        <f t="shared" si="3"/>
+        <v>14.571428571428571</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="E31" s="1">
+        <v>29</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="0"/>
+        <v>-14</v>
+      </c>
+      <c r="G31" s="1">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="P31" s="1">
+        <v>29</v>
+      </c>
+      <c r="Q31" s="1">
+        <f t="shared" si="2"/>
+        <v>-14.571428571428571</v>
+      </c>
+      <c r="R31" s="1">
+        <f t="shared" si="3"/>
+        <v>14.428571428571429</v>
+      </c>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="E32" s="1">
+        <v>30</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="0"/>
+        <v>-15.142857142857142</v>
+      </c>
+      <c r="G32" s="1">
+        <f t="shared" si="1"/>
+        <v>14.857142857142858</v>
+      </c>
+      <c r="P32" s="1">
+        <v>30</v>
+      </c>
+      <c r="Q32" s="1">
+        <f t="shared" si="2"/>
+        <v>-15.714285714285714</v>
+      </c>
+      <c r="R32" s="1">
+        <f t="shared" si="3"/>
+        <v>14.285714285714286</v>
+      </c>
+    </row>
+    <row r="33" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E33" s="1">
+        <v>31</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="0"/>
+        <v>-16.285714285714285</v>
+      </c>
+      <c r="G33" s="1">
+        <f t="shared" si="1"/>
+        <v>14.714285714285715</v>
+      </c>
+      <c r="P33" s="1">
+        <v>31</v>
+      </c>
+      <c r="Q33" s="1">
+        <f t="shared" si="2"/>
+        <v>-16.857142857142858</v>
+      </c>
+      <c r="R33" s="1">
+        <f t="shared" si="3"/>
+        <v>14.142857142857142</v>
+      </c>
+    </row>
+    <row r="34" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E34" s="1">
+        <v>32</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" si="0"/>
+        <v>-17.428571428571427</v>
+      </c>
+      <c r="G34" s="1">
+        <f t="shared" si="1"/>
+        <v>14.571428571428573</v>
+      </c>
+      <c r="P34" s="1">
+        <v>32</v>
+      </c>
+      <c r="Q34" s="1">
+        <f t="shared" si="2"/>
+        <v>-18</v>
+      </c>
+      <c r="R34" s="1">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E35" s="1">
+        <v>33</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="0"/>
+        <v>-18.571428571428573</v>
+      </c>
+      <c r="G35" s="1">
+        <f t="shared" si="1"/>
+        <v>14.428571428571427</v>
+      </c>
+      <c r="P35" s="1">
+        <v>33</v>
+      </c>
+      <c r="Q35" s="1">
+        <f t="shared" si="2"/>
+        <v>-19.142857142857142</v>
+      </c>
+      <c r="R35" s="1">
+        <f t="shared" si="3"/>
+        <v>13.857142857142858</v>
+      </c>
+    </row>
+    <row r="36" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E36" s="1">
+        <v>34</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="0"/>
+        <v>-19.714285714285715</v>
+      </c>
+      <c r="G36" s="1">
+        <f t="shared" si="1"/>
+        <v>14.285714285714285</v>
+      </c>
+      <c r="P36" s="1">
+        <v>34</v>
+      </c>
+      <c r="Q36" s="1">
+        <f t="shared" si="2"/>
+        <v>-20.285714285714285</v>
+      </c>
+      <c r="R36" s="1">
+        <f t="shared" si="3"/>
+        <v>13.714285714285715</v>
+      </c>
+    </row>
+    <row r="37" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E37" s="1">
+        <v>35</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="0"/>
+        <v>-20.857142857142858</v>
+      </c>
+      <c r="G37" s="1">
+        <f t="shared" si="1"/>
+        <v>14.142857142857142</v>
+      </c>
+      <c r="P37" s="1">
+        <v>35</v>
+      </c>
+      <c r="Q37" s="1">
+        <f t="shared" si="2"/>
+        <v>-21.428571428571427</v>
+      </c>
+      <c r="R37" s="1">
+        <f t="shared" si="3"/>
+        <v>13.571428571428573</v>
+      </c>
+    </row>
+    <row r="38" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E38" s="1">
+        <v>36</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="0"/>
+        <v>-22</v>
+      </c>
+      <c r="G38" s="1">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="P38" s="1">
+        <v>36</v>
+      </c>
+      <c r="Q38" s="1">
+        <f t="shared" si="2"/>
+        <v>-22.571428571428573</v>
+      </c>
+      <c r="R38" s="1">
+        <f t="shared" si="3"/>
+        <v>13.428571428571427</v>
+      </c>
+    </row>
+    <row r="39" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E39" s="1">
+        <v>37</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="0"/>
+        <v>-23.142857142857142</v>
+      </c>
+      <c r="G39" s="1">
+        <f t="shared" si="1"/>
+        <v>13.857142857142858</v>
+      </c>
+      <c r="I39" s="1">
+        <v>9</v>
+      </c>
+      <c r="J39" s="1">
+        <v>10</v>
+      </c>
+      <c r="K39">
+        <v>11</v>
+      </c>
+      <c r="P39" s="1">
+        <v>37</v>
+      </c>
+      <c r="Q39" s="1">
+        <f t="shared" si="2"/>
+        <v>-23.714285714285715</v>
+      </c>
+      <c r="R39" s="1">
+        <f t="shared" si="3"/>
+        <v>13.285714285714285</v>
+      </c>
+    </row>
+    <row r="40" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E40" s="1">
+        <v>38</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="0"/>
+        <v>-24.285714285714285</v>
+      </c>
+      <c r="G40" s="1">
+        <f t="shared" si="1"/>
+        <v>13.714285714285715</v>
+      </c>
+      <c r="I40" s="1">
+        <v>0</v>
+      </c>
+      <c r="J40" s="1">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40" s="1">
+        <v>12</v>
+      </c>
+      <c r="M40">
+        <v>13</v>
+      </c>
+      <c r="P40" s="1">
+        <v>38</v>
+      </c>
+      <c r="Q40" s="1">
+        <f t="shared" si="2"/>
+        <v>-24.857142857142858</v>
+      </c>
+      <c r="R40" s="1">
+        <f t="shared" si="3"/>
+        <v>13.142857142857142</v>
+      </c>
+    </row>
+    <row r="41" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E41" s="1">
+        <v>39</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="0"/>
+        <v>-25.428571428571427</v>
+      </c>
+      <c r="G41" s="1">
+        <f t="shared" si="1"/>
+        <v>13.571428571428573</v>
+      </c>
+      <c r="L41" s="1">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="P41" s="1">
+        <v>39</v>
+      </c>
+      <c r="Q41" s="1">
+        <f t="shared" si="2"/>
+        <v>-26</v>
+      </c>
+      <c r="R41" s="1">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E42" s="1">
+        <v>40</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="0"/>
+        <v>-26.571428571428573</v>
+      </c>
+      <c r="G42" s="1">
+        <f t="shared" si="1"/>
+        <v>13.428571428571427</v>
+      </c>
+      <c r="P42" s="1">
+        <v>40</v>
+      </c>
+      <c r="Q42" s="1">
+        <f t="shared" si="2"/>
+        <v>-27.142857142857142</v>
+      </c>
+      <c r="R42" s="1">
+        <f t="shared" si="3"/>
+        <v>12.857142857142858</v>
+      </c>
+    </row>
+    <row r="43" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E43" s="1">
+        <v>41</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="0"/>
+        <v>-27.714285714285715</v>
+      </c>
+      <c r="G43" s="1">
+        <f t="shared" si="1"/>
+        <v>13.285714285714285</v>
+      </c>
+      <c r="P43" s="1">
+        <v>41</v>
+      </c>
+      <c r="Q43" s="1">
+        <f t="shared" si="2"/>
+        <v>-28.285714285714285</v>
+      </c>
+      <c r="R43" s="1">
+        <f t="shared" si="3"/>
+        <v>12.714285714285715</v>
+      </c>
+    </row>
+    <row r="44" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E44" s="1">
+        <v>42</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="0"/>
+        <v>-28.857142857142858</v>
+      </c>
+      <c r="G44" s="1">
+        <f t="shared" si="1"/>
+        <v>13.142857142857142</v>
+      </c>
+      <c r="P44" s="1">
+        <v>42</v>
+      </c>
+      <c r="Q44" s="1">
+        <f t="shared" si="2"/>
+        <v>-29.428571428571427</v>
+      </c>
+      <c r="R44" s="1">
+        <f t="shared" si="3"/>
+        <v>12.571428571428573</v>
+      </c>
+    </row>
+    <row r="45" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E45" s="1">
+        <v>43</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="0"/>
+        <v>-30</v>
+      </c>
+      <c r="G45" s="1">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="P45" s="1">
+        <v>43</v>
+      </c>
+      <c r="Q45" s="1">
+        <f t="shared" si="2"/>
+        <v>-30.571428571428573</v>
+      </c>
+      <c r="R45" s="1">
+        <f t="shared" si="3"/>
+        <v>12.428571428571427</v>
+      </c>
+    </row>
+    <row r="46" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E46" s="1">
+        <v>44</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="0"/>
+        <v>-31.142857142857142</v>
+      </c>
+      <c r="G46" s="1">
+        <f t="shared" si="1"/>
+        <v>12.857142857142858</v>
+      </c>
+      <c r="P46" s="1">
+        <v>44</v>
+      </c>
+      <c r="Q46" s="1">
+        <f t="shared" si="2"/>
+        <v>-31.714285714285715</v>
+      </c>
+      <c r="R46" s="1">
+        <f t="shared" si="3"/>
+        <v>12.285714285714285</v>
+      </c>
+    </row>
+    <row r="47" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E47" s="1">
+        <v>45</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="0"/>
+        <v>-32.285714285714285</v>
+      </c>
+      <c r="G47" s="1">
+        <f t="shared" si="1"/>
+        <v>12.714285714285715</v>
+      </c>
+      <c r="P47" s="1">
+        <v>45</v>
+      </c>
+      <c r="Q47" s="1">
+        <f t="shared" si="2"/>
+        <v>-32.857142857142854</v>
+      </c>
+      <c r="R47" s="1">
+        <f t="shared" si="3"/>
+        <v>12.142857142857146</v>
+      </c>
+    </row>
+    <row r="48" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E48" s="1">
+        <v>46</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="0"/>
+        <v>-33.428571428571431</v>
+      </c>
+      <c r="G48" s="1">
+        <f t="shared" si="1"/>
+        <v>12.571428571428569</v>
+      </c>
+      <c r="P48" s="1">
+        <v>46</v>
+      </c>
+      <c r="Q48" s="1">
+        <f t="shared" si="2"/>
+        <v>-34</v>
+      </c>
+      <c r="R48" s="1">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E49" s="1">
+        <v>47</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="0"/>
+        <v>-34.571428571428569</v>
+      </c>
+      <c r="G49" s="1">
+        <f t="shared" si="1"/>
+        <v>12.428571428571431</v>
+      </c>
+      <c r="P49" s="1">
+        <v>47</v>
+      </c>
+      <c r="Q49" s="1">
+        <f t="shared" si="2"/>
+        <v>-35.142857142857146</v>
+      </c>
+      <c r="R49" s="1">
+        <f t="shared" si="3"/>
+        <v>11.857142857142854</v>
+      </c>
+    </row>
+    <row r="50" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E50" s="1">
+        <v>48</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="0"/>
+        <v>-35.714285714285715</v>
+      </c>
+      <c r="G50" s="1">
+        <f t="shared" si="1"/>
+        <v>12.285714285714285</v>
+      </c>
+      <c r="P50" s="1">
+        <v>48</v>
+      </c>
+      <c r="Q50" s="1">
+        <f t="shared" si="2"/>
+        <v>-36.285714285714285</v>
+      </c>
+      <c r="R50" s="1">
+        <f t="shared" si="3"/>
+        <v>11.714285714285715</v>
+      </c>
+    </row>
+    <row r="51" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E51" s="1">
+        <v>49</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="0"/>
+        <v>-36.857142857142854</v>
+      </c>
+      <c r="G51" s="1">
+        <f t="shared" si="1"/>
+        <v>12.142857142857146</v>
+      </c>
+      <c r="P51" s="1">
+        <v>49</v>
+      </c>
+      <c r="Q51" s="1">
+        <f t="shared" si="2"/>
+        <v>-37.428571428571431</v>
+      </c>
+      <c r="R51" s="1">
+        <f t="shared" si="3"/>
+        <v>11.571428571428569</v>
+      </c>
+    </row>
+    <row r="52" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E52" s="1">
+        <v>50</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="0"/>
+        <v>-38</v>
+      </c>
+      <c r="G52" s="1">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="P52" s="1">
+        <v>50</v>
+      </c>
+      <c r="Q52" s="1">
+        <f t="shared" si="2"/>
+        <v>-38.571428571428569</v>
+      </c>
+      <c r="R52" s="1">
+        <f t="shared" si="3"/>
+        <v>11.428571428571431</v>
+      </c>
+    </row>
+    <row r="53" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E53" s="1">
+        <v>51</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="0"/>
+        <v>-39.142857142857146</v>
+      </c>
+      <c r="G53" s="1">
+        <f t="shared" si="1"/>
+        <v>11.857142857142854</v>
+      </c>
+      <c r="P53" s="1">
+        <v>51</v>
+      </c>
+      <c r="Q53" s="1">
+        <f t="shared" si="2"/>
+        <v>-39.714285714285715</v>
+      </c>
+      <c r="R53" s="1">
+        <f t="shared" si="3"/>
+        <v>11.285714285714285</v>
+      </c>
+    </row>
+    <row r="54" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E54" s="1">
+        <v>52</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="0"/>
+        <v>-40.285714285714285</v>
+      </c>
+      <c r="G54" s="1">
+        <f t="shared" si="1"/>
+        <v>11.714285714285715</v>
+      </c>
+      <c r="P54" s="1">
+        <v>52</v>
+      </c>
+      <c r="Q54" s="1">
+        <f t="shared" si="2"/>
+        <v>-40.857142857142854</v>
+      </c>
+      <c r="R54" s="1">
+        <f t="shared" si="3"/>
+        <v>11.142857142857146</v>
+      </c>
+    </row>
+    <row r="55" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E55" s="1">
+        <v>53</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="0"/>
+        <v>-41.428571428571431</v>
+      </c>
+      <c r="G55" s="1">
+        <f t="shared" si="1"/>
+        <v>11.571428571428569</v>
+      </c>
+      <c r="P55" s="1">
+        <v>53</v>
+      </c>
+      <c r="Q55" s="1">
+        <f t="shared" si="2"/>
+        <v>-42</v>
+      </c>
+      <c r="R55" s="1">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E56" s="1">
+        <v>54</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="0"/>
+        <v>-42.571428571428569</v>
+      </c>
+      <c r="G56" s="1">
+        <f t="shared" si="1"/>
+        <v>11.428571428571431</v>
+      </c>
+      <c r="P56" s="1">
+        <v>54</v>
+      </c>
+      <c r="Q56" s="1">
+        <f t="shared" si="2"/>
+        <v>-43.142857142857146</v>
+      </c>
+      <c r="R56" s="1">
+        <f t="shared" si="3"/>
+        <v>10.857142857142854</v>
+      </c>
+    </row>
+    <row r="57" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E57" s="1">
+        <v>55</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="0"/>
+        <v>-43.714285714285715</v>
+      </c>
+      <c r="G57" s="1">
+        <f t="shared" si="1"/>
+        <v>11.285714285714285</v>
+      </c>
+      <c r="P57" s="1">
+        <v>55</v>
+      </c>
+      <c r="Q57" s="1">
+        <f t="shared" si="2"/>
+        <v>-44.285714285714285</v>
+      </c>
+      <c r="R57" s="1">
+        <f t="shared" si="3"/>
+        <v>10.714285714285715</v>
+      </c>
+    </row>
+    <row r="58" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E58" s="1">
+        <v>56</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="0"/>
+        <v>-44.857142857142854</v>
+      </c>
+      <c r="G58" s="1">
+        <f t="shared" si="1"/>
+        <v>11.142857142857146</v>
+      </c>
+      <c r="P58" s="1">
+        <v>56</v>
+      </c>
+      <c r="Q58" s="1">
+        <f t="shared" si="2"/>
+        <v>-45.428571428571431</v>
+      </c>
+      <c r="R58" s="1">
+        <f t="shared" si="3"/>
+        <v>10.571428571428569</v>
+      </c>
+    </row>
+    <row r="59" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E59" s="1">
+        <v>57</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="0"/>
+        <v>-46</v>
+      </c>
+      <c r="G59" s="1">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="P59" s="1">
+        <v>57</v>
+      </c>
+      <c r="Q59" s="1">
+        <f t="shared" si="2"/>
+        <v>-46.571428571428569</v>
+      </c>
+      <c r="R59" s="1">
+        <f t="shared" si="3"/>
+        <v>10.428571428571431</v>
+      </c>
+    </row>
+    <row r="60" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E60" s="1">
+        <v>58</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" si="0"/>
+        <v>-47.142857142857146</v>
+      </c>
+      <c r="G60" s="1">
+        <f t="shared" si="1"/>
+        <v>10.857142857142854</v>
+      </c>
+      <c r="P60" s="1">
+        <v>58</v>
+      </c>
+      <c r="Q60" s="1">
+        <f t="shared" si="2"/>
+        <v>-47.714285714285715</v>
+      </c>
+      <c r="R60" s="1">
+        <f t="shared" si="3"/>
+        <v>10.285714285714285</v>
+      </c>
+    </row>
+    <row r="61" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E61" s="1">
+        <v>59</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" si="0"/>
+        <v>-48.285714285714285</v>
+      </c>
+      <c r="G61" s="1">
+        <f t="shared" si="1"/>
+        <v>10.714285714285715</v>
+      </c>
+      <c r="P61" s="1">
+        <v>59</v>
+      </c>
+      <c r="Q61" s="1">
+        <f t="shared" si="2"/>
+        <v>-48.857142857142854</v>
+      </c>
+      <c r="R61" s="1">
+        <f t="shared" si="3"/>
+        <v>10.142857142857146</v>
+      </c>
+    </row>
+    <row r="62" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E62" s="1">
+        <v>60</v>
+      </c>
+      <c r="F62" s="1">
+        <f t="shared" si="0"/>
+        <v>-49.428571428571431</v>
+      </c>
+      <c r="G62" s="1">
+        <f t="shared" si="1"/>
+        <v>10.571428571428569</v>
+      </c>
+      <c r="P62" s="1">
+        <v>60</v>
+      </c>
+      <c r="Q62" s="1">
+        <f t="shared" si="2"/>
+        <v>-50</v>
+      </c>
+      <c r="R62" s="1">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E63" s="1">
+        <v>61</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="0"/>
+        <v>-50.571428571428569</v>
+      </c>
+      <c r="G63" s="1">
+        <f t="shared" si="1"/>
+        <v>10.428571428571431</v>
+      </c>
+      <c r="P63" s="1">
+        <v>61</v>
+      </c>
+      <c r="Q63" s="1">
+        <f t="shared" si="2"/>
+        <v>-51.142857142857146</v>
+      </c>
+      <c r="R63" s="1">
+        <f t="shared" si="3"/>
+        <v>9.8571428571428541</v>
+      </c>
+    </row>
+    <row r="64" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E64" s="1">
+        <v>62</v>
+      </c>
+      <c r="F64" s="1">
+        <f t="shared" si="0"/>
+        <v>-51.714285714285715</v>
+      </c>
+      <c r="G64" s="1">
+        <f t="shared" si="1"/>
+        <v>10.285714285714285</v>
+      </c>
+      <c r="P64" s="1">
+        <v>62</v>
+      </c>
+      <c r="Q64" s="1">
+        <f t="shared" si="2"/>
+        <v>-52.285714285714285</v>
+      </c>
+      <c r="R64" s="1">
+        <f t="shared" si="3"/>
+        <v>9.7142857142857153</v>
+      </c>
+    </row>
+    <row r="65" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E65" s="1">
+        <v>63</v>
+      </c>
+      <c r="F65" s="1">
+        <f t="shared" si="0"/>
+        <v>-52.857142857142854</v>
+      </c>
+      <c r="G65" s="1">
+        <f t="shared" si="1"/>
+        <v>10.142857142857146</v>
+      </c>
+      <c r="P65" s="1">
+        <v>63</v>
+      </c>
+      <c r="Q65" s="1">
+        <f t="shared" si="2"/>
+        <v>-53.428571428571431</v>
+      </c>
+      <c r="R65" s="1">
+        <f t="shared" si="3"/>
+        <v>9.5714285714285694</v>
+      </c>
+    </row>
+    <row r="66" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E66" s="1">
+        <v>64</v>
+      </c>
+      <c r="F66" s="1">
+        <f t="shared" si="0"/>
+        <v>-54</v>
+      </c>
+      <c r="G66" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="P66" s="1">
+        <v>64</v>
+      </c>
+      <c r="Q66" s="1">
+        <f t="shared" si="2"/>
+        <v>-54.571428571428569</v>
+      </c>
+      <c r="R66" s="1">
+        <f t="shared" si="3"/>
+        <v>9.4285714285714306</v>
+      </c>
+    </row>
+    <row r="67" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E67" s="1">
+        <v>65</v>
+      </c>
+      <c r="F67" s="1">
+        <f t="shared" si="0"/>
+        <v>-55.142857142857146</v>
+      </c>
+      <c r="G67" s="1">
+        <f t="shared" si="1"/>
+        <v>9.8571428571428541</v>
+      </c>
+      <c r="P67" s="1">
+        <v>65</v>
+      </c>
+      <c r="Q67" s="1">
+        <f t="shared" si="2"/>
+        <v>-55.714285714285715</v>
+      </c>
+      <c r="R67" s="1">
+        <f t="shared" si="3"/>
+        <v>9.2857142857142847</v>
+      </c>
+    </row>
+    <row r="68" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E68" s="1">
+        <v>66</v>
+      </c>
+      <c r="F68" s="1">
+        <f t="shared" ref="F68:F77" si="5">($D$3-(8*E68))/7</f>
+        <v>-56.285714285714285</v>
+      </c>
+      <c r="G68" s="1">
+        <f t="shared" ref="G68:G77" si="6">E68+F68</f>
+        <v>9.7142857142857153</v>
+      </c>
+      <c r="P68" s="1">
+        <v>66</v>
+      </c>
+      <c r="Q68" s="1">
+        <f t="shared" ref="Q68:Q77" si="7">($O$3-(8*P68))/7</f>
+        <v>-56.857142857142854</v>
+      </c>
+      <c r="R68" s="1">
+        <f t="shared" ref="R68:R77" si="8">P68+Q68</f>
+        <v>9.1428571428571459</v>
+      </c>
+    </row>
+    <row r="69" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E69" s="1">
+        <v>67</v>
+      </c>
+      <c r="F69" s="1">
+        <f t="shared" si="5"/>
+        <v>-57.428571428571431</v>
+      </c>
+      <c r="G69" s="1">
+        <f t="shared" si="6"/>
+        <v>9.5714285714285694</v>
+      </c>
+      <c r="P69" s="1">
+        <v>67</v>
+      </c>
+      <c r="Q69" s="1">
+        <f t="shared" si="7"/>
+        <v>-58</v>
+      </c>
+      <c r="R69" s="1">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E70" s="1">
+        <v>68</v>
+      </c>
+      <c r="F70" s="1">
+        <f t="shared" si="5"/>
+        <v>-58.571428571428569</v>
+      </c>
+      <c r="G70" s="1">
+        <f t="shared" si="6"/>
+        <v>9.4285714285714306</v>
+      </c>
+      <c r="P70" s="1">
+        <v>68</v>
+      </c>
+      <c r="Q70" s="1">
+        <f t="shared" si="7"/>
+        <v>-59.142857142857146</v>
+      </c>
+      <c r="R70" s="1">
+        <f t="shared" si="8"/>
+        <v>8.8571428571428541</v>
+      </c>
+    </row>
+    <row r="71" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E71" s="1">
+        <v>69</v>
+      </c>
+      <c r="F71" s="1">
+        <f t="shared" si="5"/>
+        <v>-59.714285714285715</v>
+      </c>
+      <c r="G71" s="1">
+        <f t="shared" si="6"/>
+        <v>9.2857142857142847</v>
+      </c>
+      <c r="P71" s="1">
+        <v>69</v>
+      </c>
+      <c r="Q71" s="1">
+        <f t="shared" si="7"/>
+        <v>-60.285714285714285</v>
+      </c>
+      <c r="R71" s="1">
+        <f t="shared" si="8"/>
+        <v>8.7142857142857153</v>
+      </c>
+    </row>
+    <row r="72" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E72" s="1">
+        <v>70</v>
+      </c>
+      <c r="F72" s="1">
+        <f t="shared" si="5"/>
+        <v>-60.857142857142854</v>
+      </c>
+      <c r="G72" s="1">
+        <f t="shared" si="6"/>
+        <v>9.1428571428571459</v>
+      </c>
+      <c r="P72" s="1">
+        <v>70</v>
+      </c>
+      <c r="Q72" s="1">
+        <f t="shared" si="7"/>
+        <v>-61.428571428571431</v>
+      </c>
+      <c r="R72" s="1">
+        <f t="shared" si="8"/>
+        <v>8.5714285714285694</v>
+      </c>
+    </row>
+    <row r="73" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E73" s="1">
+        <v>71</v>
+      </c>
+      <c r="F73" s="1">
+        <f t="shared" si="5"/>
+        <v>-62</v>
+      </c>
+      <c r="G73" s="1">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="P73" s="1">
+        <v>71</v>
+      </c>
+      <c r="Q73" s="1">
+        <f t="shared" si="7"/>
+        <v>-62.571428571428569</v>
+      </c>
+      <c r="R73" s="1">
+        <f t="shared" si="8"/>
+        <v>8.4285714285714306</v>
+      </c>
+    </row>
+    <row r="74" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E74" s="1">
+        <v>72</v>
+      </c>
+      <c r="F74" s="1">
+        <f t="shared" si="5"/>
+        <v>-63.142857142857146</v>
+      </c>
+      <c r="G74" s="1">
+        <f t="shared" si="6"/>
+        <v>8.8571428571428541</v>
+      </c>
+      <c r="P74" s="1">
+        <v>72</v>
+      </c>
+      <c r="Q74" s="1">
+        <f t="shared" si="7"/>
+        <v>-63.714285714285715</v>
+      </c>
+      <c r="R74" s="1">
+        <f t="shared" si="8"/>
+        <v>8.2857142857142847</v>
+      </c>
+    </row>
+    <row r="75" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E75" s="1">
+        <v>73</v>
+      </c>
+      <c r="F75" s="1">
+        <f t="shared" si="5"/>
+        <v>-64.285714285714292</v>
+      </c>
+      <c r="G75" s="1">
+        <f t="shared" si="6"/>
+        <v>8.7142857142857082</v>
+      </c>
+      <c r="P75" s="1">
+        <v>73</v>
+      </c>
+      <c r="Q75" s="1">
+        <f t="shared" si="7"/>
+        <v>-64.857142857142861</v>
+      </c>
+      <c r="R75" s="1">
+        <f t="shared" si="8"/>
+        <v>8.1428571428571388</v>
+      </c>
+    </row>
+    <row r="76" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E76" s="1">
+        <v>74</v>
+      </c>
+      <c r="F76" s="1">
+        <f t="shared" si="5"/>
+        <v>-65.428571428571431</v>
+      </c>
+      <c r="G76" s="1">
+        <f t="shared" si="6"/>
+        <v>8.5714285714285694</v>
+      </c>
+      <c r="P76" s="1">
+        <v>74</v>
+      </c>
+      <c r="Q76" s="1">
+        <f t="shared" si="7"/>
+        <v>-66</v>
+      </c>
+      <c r="R76" s="1">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E77" s="1">
+        <v>75</v>
+      </c>
+      <c r="F77" s="1">
+        <f t="shared" si="5"/>
+        <v>-66.571428571428569</v>
+      </c>
+      <c r="G77" s="1">
+        <f t="shared" si="6"/>
+        <v>8.4285714285714306</v>
+      </c>
+      <c r="P77" s="1">
+        <v>75</v>
+      </c>
+      <c r="Q77" s="1">
+        <f t="shared" si="7"/>
+        <v>-67.142857142857139</v>
+      </c>
+      <c r="R77" s="1">
+        <f t="shared" si="8"/>
+        <v>7.8571428571428612</v>
+      </c>
+    </row>
+    <row r="81" spans="3:64" x14ac:dyDescent="0.25">
+      <c r="C81">
+        <v>3</v>
+      </c>
+      <c r="D81" s="1">
+        <v>4</v>
+      </c>
+      <c r="E81" s="1">
+        <v>5</v>
+      </c>
+      <c r="F81">
+        <v>6</v>
+      </c>
+      <c r="G81" s="1">
+        <v>7</v>
+      </c>
+      <c r="H81">
+        <v>8</v>
+      </c>
+      <c r="N81" s="1">
+        <v>14</v>
+      </c>
+      <c r="O81" s="1">
+        <v>15</v>
+      </c>
+      <c r="P81">
+        <v>16</v>
+      </c>
+      <c r="Q81" s="1">
+        <v>17</v>
+      </c>
+      <c r="R81">
+        <v>18</v>
+      </c>
+      <c r="S81" s="1">
+        <v>19</v>
+      </c>
+      <c r="T81" s="1">
+        <v>20</v>
+      </c>
+      <c r="U81">
+        <v>21</v>
+      </c>
+      <c r="V81" s="1">
+        <v>22</v>
+      </c>
+      <c r="W81">
+        <v>23</v>
+      </c>
+      <c r="X81" s="1">
+        <v>24</v>
+      </c>
+      <c r="Y81" s="1">
+        <v>25</v>
+      </c>
+      <c r="Z81">
+        <v>26</v>
+      </c>
+      <c r="AA81" s="1">
+        <v>27</v>
+      </c>
+      <c r="AB81">
+        <v>28</v>
+      </c>
+      <c r="AC81" s="1">
+        <v>29</v>
+      </c>
+      <c r="AD81" s="1">
+        <v>30</v>
+      </c>
+      <c r="AE81">
+        <v>31</v>
+      </c>
+      <c r="AF81" s="1">
+        <v>32</v>
+      </c>
+      <c r="AG81">
+        <v>33</v>
+      </c>
+      <c r="AH81" s="1">
+        <v>34</v>
+      </c>
+      <c r="AI81" s="1">
+        <v>35</v>
+      </c>
+      <c r="AJ81">
+        <v>36</v>
+      </c>
+      <c r="AK81" s="1">
+        <v>37</v>
+      </c>
+      <c r="AL81">
+        <v>38</v>
+      </c>
+      <c r="AM81" s="1">
+        <v>39</v>
+      </c>
+      <c r="AN81" s="1">
+        <v>40</v>
+      </c>
+      <c r="AO81">
+        <v>41</v>
+      </c>
+      <c r="AP81" s="1">
+        <v>42</v>
+      </c>
+      <c r="AQ81">
+        <v>43</v>
+      </c>
+      <c r="AR81" s="1">
+        <v>44</v>
+      </c>
+      <c r="AS81" s="1">
+        <v>45</v>
+      </c>
+      <c r="AT81">
+        <v>46</v>
+      </c>
+      <c r="AU81" s="1">
+        <v>47</v>
+      </c>
+      <c r="AV81">
+        <v>48</v>
+      </c>
+      <c r="AW81" s="1">
+        <v>49</v>
+      </c>
+      <c r="AX81" s="1">
+        <v>50</v>
+      </c>
+      <c r="AY81">
+        <v>51</v>
+      </c>
+      <c r="AZ81" s="1">
+        <v>52</v>
+      </c>
+      <c r="BA81">
+        <v>53</v>
+      </c>
+      <c r="BB81" s="1">
+        <v>54</v>
+      </c>
+      <c r="BC81" s="1">
+        <v>55</v>
+      </c>
+      <c r="BD81">
+        <v>56</v>
+      </c>
+      <c r="BE81" s="1">
+        <v>57</v>
+      </c>
+      <c r="BF81">
+        <v>58</v>
+      </c>
+      <c r="BG81" s="1">
+        <v>59</v>
+      </c>
+      <c r="BH81" s="1">
+        <v>60</v>
+      </c>
+      <c r="BI81">
+        <v>61</v>
+      </c>
+      <c r="BJ81" s="1">
+        <v>62</v>
+      </c>
+      <c r="BK81">
+        <v>63</v>
+      </c>
+      <c r="BL81" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="82" spans="3:64" x14ac:dyDescent="0.25">
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82" s="1">
+        <v>0</v>
+      </c>
+      <c r="E82" s="1">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82" s="1">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="N82" s="1">
+        <v>0</v>
+      </c>
+      <c r="O82" s="1">
+        <v>0</v>
+      </c>
+      <c r="P82">
+        <v>0</v>
+      </c>
+      <c r="Q82" s="1">
+        <v>0</v>
+      </c>
+      <c r="R82">
+        <v>0</v>
+      </c>
+      <c r="S82" s="1">
+        <v>0</v>
+      </c>
+      <c r="T82" s="1">
+        <v>0</v>
+      </c>
+      <c r="U82">
+        <v>0</v>
+      </c>
+      <c r="V82" s="1">
+        <v>0</v>
+      </c>
+      <c r="W82">
+        <v>0</v>
+      </c>
+      <c r="X82" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y82" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z82">
+        <v>0</v>
+      </c>
+      <c r="AA82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB82">
+        <v>0</v>
+      </c>
+      <c r="AC82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE82">
+        <v>0</v>
+      </c>
+      <c r="AF82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG82">
+        <v>0</v>
+      </c>
+      <c r="AH82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ82">
+        <v>0</v>
+      </c>
+      <c r="AK82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL82">
+        <v>0</v>
+      </c>
+      <c r="AM82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO82">
+        <v>0</v>
+      </c>
+      <c r="AP82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ82">
+        <v>0</v>
+      </c>
+      <c r="AR82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT82">
+        <v>0</v>
+      </c>
+      <c r="AU82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV82">
+        <v>0</v>
+      </c>
+      <c r="AW82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY82">
+        <v>0</v>
+      </c>
+      <c r="AZ82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA82">
+        <v>0</v>
+      </c>
+      <c r="BB82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD82">
+        <v>0</v>
+      </c>
+      <c r="BE82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF82">
+        <v>1</v>
+      </c>
+      <c r="BG82" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH82" s="1">
+        <v>1</v>
+      </c>
+      <c r="BI82">
+        <v>1</v>
+      </c>
+      <c r="BJ82" s="1">
+        <v>1</v>
+      </c>
+      <c r="BK82">
+        <v>1</v>
+      </c>
+      <c r="BL82" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I3:J22">
+    <sortCondition descending="1" ref="J3:J22"/>
   </sortState>
   <mergeCells count="4">
     <mergeCell ref="D1:G1"/>

</xml_diff>